<commit_message>
Actualizacion BOM MK1 RP2040
</commit_message>
<xml_diff>
--- a/02.Hardware/MK1-RP2040/01.EDCPSU/BOM/EDCPSU_MK1_RP2040_BOM-SETI.xlsx
+++ b/02.Hardware/MK1-RP2040/01.EDCPSU/BOM/EDCPSU_MK1_RP2040_BOM-SETI.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Team Dropbox\JRODRIGUEZ\Repositorios\11.MK1\02.Hardware\MK1-RP2040\01.EDCPSU\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC428E32-E1F1-48B9-9BF5-0B7C78098F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9A3C8F-3C02-4429-8A1B-4D619D28013D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19215" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="18900" yWindow="0" windowWidth="10005" windowHeight="15585" activeTab="1" xr2:uid="{CDEA638F-CF3E-43EC-96DC-54CE86003FCC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CDEA638F-CF3E-43EC-96DC-54CE86003FCC}"/>
   </bookViews>
   <sheets>
     <sheet name="EDCPSUMK1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="249">
   <si>
     <t>Qty</t>
   </si>
@@ -196,9 +196,6 @@
     <t>DO-214AB</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
     <t>Display</t>
   </si>
   <si>
@@ -433,12 +430,6 @@
     <t>150K</t>
   </si>
   <si>
-    <t>R38, R63</t>
-  </si>
-  <si>
-    <t>27R</t>
-  </si>
-  <si>
     <t>27K</t>
   </si>
   <si>
@@ -733,15 +724,6 @@
     <t>TVS 18V 400W Unidirectional</t>
   </si>
   <si>
-    <t>https://www.digikey.es/en/products/detail/littelfuse-inc/SMAJ24A/762288</t>
-  </si>
-  <si>
-    <t>ESD Suppressors / TVS Diodes 24volts 5uA 10.3 Amps UNI-Dir</t>
-  </si>
-  <si>
-    <t>SMAJ24A</t>
-  </si>
-  <si>
     <t>COST (500pcs)</t>
   </si>
   <si>
@@ -791,6 +773,12 @@
   </si>
   <si>
     <t>R1,R32, R39, R40, R42, R66</t>
+  </si>
+  <si>
+    <t>BOM VERSION v1</t>
+  </si>
+  <si>
+    <t>MK1-RP2040</t>
   </si>
   <si>
     <t>Modificaciones frente a la v4 de la MK2-RP2040:
@@ -808,13 +796,9 @@
 Se elimina la posicion 59, part R62
 Se elimina la posicion 64, part RSENSE
 Se elimina la posicion 68, part U10
-Se elimina la posicion 77, part U9</t>
-  </si>
-  <si>
-    <t>BOM VERSION v1</t>
-  </si>
-  <si>
-    <t>MK1-RP2040</t>
+Se elimina la posicion 77, part U9
+Se elimina la posicion 16, part D1
+Se elimina la posicion 47, part R38 y R63</t>
   </si>
 </sst>
 </file>
@@ -1775,7 +1759,7 @@
     <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1943,44 +1927,38 @@
     <xf numFmtId="0" fontId="47" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="47" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="85">
@@ -2395,17 +2373,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="1">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="8" customWidth="1"/>
     <col min="2" max="2" width="4" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" style="66" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.140625" style="5" bestFit="1" customWidth="1"/>
@@ -2418,7 +2398,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="D1" s="3" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="J1"/>
     </row>
@@ -2429,26 +2409,25 @@
       <c r="J2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D3" s="67"/>
+      <c r="D3" s="65"/>
       <c r="J3"/>
     </row>
     <row r="4" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D4" s="2" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="J4"/>
     </row>
     <row r="5" spans="1:12" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="D5" s="7"/>
       <c r="G5" s="1"/>
       <c r="J5"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>0</v>
@@ -2469,21 +2448,21 @@
         <v>5</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" s="19">
         <v>2</v>
@@ -2491,20 +2470,20 @@
       <c r="C7" s="28">
         <v>1</v>
       </c>
-      <c r="D7" s="63" t="s">
-        <v>57</v>
+      <c r="D7" s="28" t="s">
+        <v>56</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I7" s="36"/>
       <c r="J7" s="58">
@@ -2515,12 +2494,12 @@
         <v>0.48</v>
       </c>
       <c r="L7" s="46" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="19">
         <v>3</v>
@@ -2528,17 +2507,17 @@
       <c r="C8" s="28">
         <v>3</v>
       </c>
-      <c r="D8" s="63" t="s">
+      <c r="D8" s="28" t="s">
         <v>35</v>
       </c>
       <c r="E8" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="F8" s="28" t="s">
-        <v>85</v>
-      </c>
       <c r="G8" s="28" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H8" s="28" t="s">
         <v>14</v>
@@ -2552,12 +2531,12 @@
         <v>0.31794</v>
       </c>
       <c r="L8" s="33" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" s="19">
         <v>4</v>
@@ -2565,17 +2544,17 @@
       <c r="C9" s="28">
         <v>0</v>
       </c>
-      <c r="D9" s="63" t="s">
-        <v>102</v>
+      <c r="D9" s="28" t="s">
+        <v>101</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F9" s="28" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H9" s="28" t="s">
         <v>14</v>
@@ -2590,7 +2569,7 @@
     </row>
     <row r="10" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B10" s="19">
         <v>5</v>
@@ -2598,17 +2577,17 @@
       <c r="C10" s="28">
         <v>32</v>
       </c>
-      <c r="D10" s="64" t="s">
-        <v>245</v>
+      <c r="D10" s="63" t="s">
+        <v>239</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F10" s="28" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H10" s="28" t="s">
         <v>14</v>
@@ -2623,7 +2602,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" s="19">
         <v>6</v>
@@ -2631,17 +2610,17 @@
       <c r="C11" s="28">
         <v>4</v>
       </c>
-      <c r="D11" s="63" t="s">
+      <c r="D11" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="62" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="62" t="s">
-        <v>88</v>
-      </c>
       <c r="F11" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H11" s="28" t="s">
         <v>14</v>
@@ -2655,12 +2634,12 @@
         <v>0.27688000000000001</v>
       </c>
       <c r="L11" s="33" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12" s="19">
         <v>7</v>
@@ -2668,17 +2647,17 @@
       <c r="C12" s="28">
         <v>2</v>
       </c>
-      <c r="D12" s="63" t="s">
-        <v>89</v>
+      <c r="D12" s="28" t="s">
+        <v>88</v>
       </c>
       <c r="E12" s="62" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F12" s="28" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H12" s="28" t="s">
         <v>14</v>
@@ -2692,12 +2671,12 @@
         <v>0.11260000000000001</v>
       </c>
       <c r="L12" s="33" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" s="19">
         <v>8</v>
@@ -2705,17 +2684,17 @@
       <c r="C13" s="28">
         <v>1</v>
       </c>
-      <c r="D13" s="63" t="s">
+      <c r="D13" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13" s="28" t="s">
         <v>90</v>
-      </c>
-      <c r="E13" s="28" t="s">
-        <v>91</v>
       </c>
       <c r="F13" s="28" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H13" s="28" t="s">
         <v>14</v>
@@ -2730,7 +2709,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B14" s="19">
         <v>9</v>
@@ -2738,17 +2717,17 @@
       <c r="C14" s="28">
         <v>1</v>
       </c>
-      <c r="D14" s="63" t="s">
+      <c r="D14" s="28" t="s">
         <v>24</v>
       </c>
       <c r="E14" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F14" s="28" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H14" s="28" t="s">
         <v>14</v>
@@ -2763,7 +2742,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B15" s="19">
         <v>10</v>
@@ -2771,17 +2750,17 @@
       <c r="C15" s="28">
         <v>1</v>
       </c>
-      <c r="D15" s="63" t="s">
+      <c r="D15" s="28" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F15" s="28" t="s">
         <v>13</v>
       </c>
       <c r="G15" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H15" s="28" t="s">
         <v>14</v>
@@ -2796,7 +2775,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" s="19">
         <v>11</v>
@@ -2804,17 +2783,17 @@
       <c r="C16" s="28">
         <v>4</v>
       </c>
-      <c r="D16" s="63" t="s">
+      <c r="D16" s="28" t="s">
         <v>27</v>
       </c>
       <c r="E16" s="62" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G16" s="28" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H16" s="28" t="s">
         <v>14</v>
@@ -2828,12 +2807,12 @@
         <v>0.49447999999999998</v>
       </c>
       <c r="L16" s="33" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B17" s="19">
         <v>12</v>
@@ -2841,17 +2820,17 @@
       <c r="C17" s="28">
         <v>0</v>
       </c>
-      <c r="D17" s="63" t="s">
+      <c r="D17" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" s="28" t="s">
         <v>94</v>
-      </c>
-      <c r="E17" s="28" t="s">
-        <v>95</v>
       </c>
       <c r="F17" s="28" t="s">
         <v>13</v>
       </c>
       <c r="G17" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H17" s="28" t="s">
         <v>14</v>
@@ -2866,7 +2845,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B18" s="19">
         <v>13</v>
@@ -2874,17 +2853,17 @@
       <c r="C18" s="28">
         <v>2</v>
       </c>
-      <c r="D18" s="63" t="s">
+      <c r="D18" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18" s="28" t="s">
         <v>96</v>
-      </c>
-      <c r="E18" s="28" t="s">
-        <v>97</v>
       </c>
       <c r="F18" s="28" t="s">
         <v>13</v>
       </c>
       <c r="G18" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H18" s="28" t="s">
         <v>14</v>
@@ -2899,7 +2878,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19" s="19">
         <v>14</v>
@@ -2907,17 +2886,17 @@
       <c r="C19" s="28">
         <v>2</v>
       </c>
-      <c r="D19" s="63" t="s">
+      <c r="D19" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" s="62" t="s">
         <v>98</v>
-      </c>
-      <c r="E19" s="62" t="s">
-        <v>99</v>
       </c>
       <c r="F19" s="28" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H19" s="28" t="s">
         <v>14</v>
@@ -2931,12 +2910,12 @@
         <v>8.5519999999999999E-2</v>
       </c>
       <c r="L19" s="33" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B20" s="19">
         <v>15</v>
@@ -2944,17 +2923,17 @@
       <c r="C20" s="28">
         <v>7</v>
       </c>
-      <c r="D20" s="63" t="s">
-        <v>246</v>
+      <c r="D20" s="28" t="s">
+        <v>240</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F20" s="28" t="s">
         <v>13</v>
       </c>
       <c r="G20" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H20" s="28" t="s">
         <v>14</v>
@@ -2968,45 +2947,26 @@
       <c r="L20" s="33"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="18" t="s">
-        <v>73</v>
+      <c r="A21" s="19" t="s">
+        <v>69</v>
       </c>
       <c r="B21" s="19">
-        <v>16</v>
-      </c>
-      <c r="C21" s="28">
-        <v>1</v>
-      </c>
-      <c r="D21" s="63" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>234</v>
-      </c>
-      <c r="F21" s="28" t="s">
-        <v>234</v>
-      </c>
-      <c r="G21" s="28" t="s">
-        <v>227</v>
-      </c>
-      <c r="H21" s="28" t="s">
-        <v>233</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C21" s="66"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="66"/>
+      <c r="G21" s="66"/>
+      <c r="H21" s="66"/>
       <c r="I21" s="37"/>
-      <c r="J21" s="58">
-        <v>0.10872</v>
-      </c>
-      <c r="K21" s="58">
-        <f t="shared" si="0"/>
-        <v>0.10872</v>
-      </c>
-      <c r="L21" s="56" t="s">
-        <v>232</v>
-      </c>
+      <c r="J21" s="58"/>
+      <c r="K21" s="58"/>
+      <c r="L21" s="56"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B22" s="19">
         <v>17</v>
@@ -3014,8 +2974,8 @@
       <c r="C22" s="28">
         <v>2</v>
       </c>
-      <c r="D22" s="63" t="s">
-        <v>161</v>
+      <c r="D22" s="28" t="s">
+        <v>158</v>
       </c>
       <c r="E22" s="28" t="s">
         <v>49</v>
@@ -3038,22 +2998,22 @@
         <v>0.22900000000000001</v>
       </c>
       <c r="L22" s="46" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B23" s="19">
         <v>18</v>
       </c>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="74"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="66"/>
       <c r="I23" s="37"/>
       <c r="J23" s="58"/>
       <c r="K23" s="58"/>
@@ -3061,7 +3021,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B24" s="19">
         <v>19</v>
@@ -3069,20 +3029,20 @@
       <c r="C24" s="28">
         <v>1</v>
       </c>
-      <c r="D24" s="63" t="s">
+      <c r="D24" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="E24" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="E24" s="28" t="s">
+      <c r="F24" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="H24" s="28" t="s">
         <v>107</v>
-      </c>
-      <c r="F24" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="G24" s="28" t="s">
-        <v>227</v>
-      </c>
-      <c r="H24" s="28" t="s">
-        <v>108</v>
       </c>
       <c r="I24" s="37"/>
       <c r="J24" s="58">
@@ -3093,12 +3053,12 @@
         <v>0.1181</v>
       </c>
       <c r="L24" s="56" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B25" s="19">
         <v>20</v>
@@ -3106,14 +3066,14 @@
       <c r="C25" s="28">
         <v>0</v>
       </c>
-      <c r="D25" s="63" t="s">
-        <v>83</v>
+      <c r="D25" s="28" t="s">
+        <v>82</v>
       </c>
       <c r="E25" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F25" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G25" s="28" t="s">
         <v>52</v>
@@ -3129,7 +3089,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B26" s="19">
         <v>21</v>
@@ -3137,20 +3097,20 @@
       <c r="C26" s="28">
         <v>1</v>
       </c>
-      <c r="D26" s="63" t="s">
-        <v>66</v>
+      <c r="D26" s="28" t="s">
+        <v>65</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F26" s="28" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="G26" s="28" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="H26" s="28" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="I26" s="37"/>
       <c r="J26" s="58">
@@ -3161,12 +3121,12 @@
         <v>0.12508</v>
       </c>
       <c r="L26" s="46" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B27" s="19">
         <v>22</v>
@@ -3174,20 +3134,20 @@
       <c r="C27" s="28">
         <v>1</v>
       </c>
-      <c r="D27" s="63" t="s">
-        <v>110</v>
+      <c r="D27" s="28" t="s">
+        <v>109</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F27" s="28" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G27" s="28" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H27" s="28" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="I27" s="38"/>
       <c r="J27" s="58">
@@ -3198,22 +3158,22 @@
         <v>8.6999999999999994E-2</v>
       </c>
       <c r="L27" s="46" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B28" s="19">
         <v>25</v>
       </c>
-      <c r="C28" s="74"/>
-      <c r="D28" s="74"/>
-      <c r="E28" s="74"/>
-      <c r="F28" s="74"/>
-      <c r="G28" s="74"/>
-      <c r="H28" s="74"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="66"/>
       <c r="I28" s="38"/>
       <c r="J28" s="58">
         <v>1.0803</v>
@@ -3223,12 +3183,12 @@
         <v>0</v>
       </c>
       <c r="L28" s="46" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B29" s="19">
         <v>26</v>
@@ -3236,17 +3196,17 @@
       <c r="C29" s="28">
         <v>1</v>
       </c>
-      <c r="D29" s="63" t="s">
-        <v>56</v>
+      <c r="D29" s="28" t="s">
+        <v>55</v>
       </c>
       <c r="E29" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="F29" s="28" t="s">
-        <v>55</v>
-      </c>
       <c r="G29" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H29" s="28"/>
       <c r="I29" s="38"/>
@@ -3259,7 +3219,7 @@
     </row>
     <row r="30" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B30" s="19">
         <v>27</v>
@@ -3267,20 +3227,20 @@
       <c r="C30" s="28">
         <v>1</v>
       </c>
-      <c r="D30" s="63" t="s">
+      <c r="D30" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="E30" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="E30" s="28" t="s">
+      <c r="F30" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="H30" s="28" t="s">
         <v>112</v>
-      </c>
-      <c r="F30" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="G30" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="H30" s="28" t="s">
-        <v>113</v>
       </c>
       <c r="I30" s="38"/>
       <c r="J30" s="58">
@@ -3291,12 +3251,12 @@
         <v>0.64117000000000002</v>
       </c>
       <c r="L30" s="56" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B31" s="19">
         <v>29</v>
@@ -3304,20 +3264,20 @@
       <c r="C31" s="28">
         <v>1</v>
       </c>
-      <c r="D31" s="63" t="s">
+      <c r="D31" s="28" t="s">
         <v>43</v>
       </c>
       <c r="E31" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F31" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="G31" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="F31" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="G31" s="28" t="s">
+      <c r="H31" s="28" t="s">
         <v>115</v>
-      </c>
-      <c r="H31" s="28" t="s">
-        <v>116</v>
       </c>
       <c r="I31" s="38"/>
       <c r="J31" s="59">
@@ -3328,12 +3288,12 @@
         <v>0.12452000000000001</v>
       </c>
       <c r="L31" s="56" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B32" s="19">
         <v>30</v>
@@ -3341,14 +3301,14 @@
       <c r="C32" s="28">
         <v>1</v>
       </c>
-      <c r="D32" s="63" t="s">
+      <c r="D32" s="28" t="s">
         <v>38</v>
       </c>
       <c r="E32" s="28" t="s">
         <v>36</v>
       </c>
       <c r="F32" s="28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G32" s="28" t="s">
         <v>37</v>
@@ -3363,12 +3323,12 @@
         <v>0.72116000000000002</v>
       </c>
       <c r="L32" s="46" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B33" s="19">
         <v>31</v>
@@ -3376,20 +3336,20 @@
       <c r="C33" s="28">
         <v>5</v>
       </c>
-      <c r="D33" s="63" t="s">
-        <v>64</v>
+      <c r="D33" s="28" t="s">
+        <v>63</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F33" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G33" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H33" s="28" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I33" s="38"/>
       <c r="J33" s="59">
@@ -3400,12 +3360,12 @@
         <v>0.11499999999999999</v>
       </c>
       <c r="L33" s="57" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B34" s="19">
         <v>32</v>
@@ -3413,20 +3373,20 @@
       <c r="C34" s="28">
         <v>1</v>
       </c>
-      <c r="D34" s="63" t="s">
+      <c r="D34" s="28" t="s">
         <v>7</v>
       </c>
       <c r="E34" s="28" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F34" s="28" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="G34" s="28" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="H34" s="28" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="I34" s="38"/>
       <c r="J34" s="59">
@@ -3437,12 +3397,12 @@
         <v>3.4189999999999998E-2</v>
       </c>
       <c r="L34" s="46" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B35" s="19">
         <v>33</v>
@@ -3450,20 +3410,20 @@
       <c r="C35" s="28">
         <v>0</v>
       </c>
-      <c r="D35" s="63" t="s">
+      <c r="D35" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E35" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="E35" s="28" t="s">
+      <c r="F35" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="G35" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="F35" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="G35" s="28" t="s">
+      <c r="H35" s="28" t="s">
         <v>120</v>
-      </c>
-      <c r="H35" s="28" t="s">
-        <v>121</v>
       </c>
       <c r="I35" s="39"/>
       <c r="J35" s="58"/>
@@ -3475,7 +3435,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B36" s="19">
         <v>34</v>
@@ -3483,20 +3443,20 @@
       <c r="C36" s="28">
         <v>1</v>
       </c>
-      <c r="D36" s="63" t="s">
+      <c r="D36" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E36" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="F36" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G36" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="H36" s="28" t="s">
         <v>60</v>
-      </c>
-      <c r="E36" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="F36" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="G36" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="H36" s="28" t="s">
-        <v>61</v>
       </c>
       <c r="I36" s="35"/>
       <c r="J36" s="58">
@@ -3507,12 +3467,12 @@
         <v>0.1341</v>
       </c>
       <c r="L36" s="46" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B37" s="19">
         <v>35</v>
@@ -3520,20 +3480,20 @@
       <c r="C37" s="28">
         <v>1</v>
       </c>
-      <c r="D37" s="63" t="s">
+      <c r="D37" s="28" t="s">
         <v>28</v>
       </c>
       <c r="E37" s="28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F37" s="28" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G37" s="28" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="H37" s="49" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="I37" s="38"/>
       <c r="J37" s="59">
@@ -3544,12 +3504,12 @@
         <v>0.12822</v>
       </c>
       <c r="L37" s="57" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B38" s="19">
         <v>36</v>
@@ -3557,20 +3517,20 @@
       <c r="C38" s="28">
         <v>3</v>
       </c>
-      <c r="D38" s="63" t="s">
-        <v>247</v>
+      <c r="D38" s="28" t="s">
+        <v>241</v>
       </c>
       <c r="E38" s="28" t="s">
         <v>32</v>
       </c>
       <c r="F38" s="28" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G38" s="28" t="s">
         <v>33</v>
       </c>
       <c r="H38" s="28" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="I38" s="38"/>
       <c r="J38" s="59">
@@ -3581,12 +3541,12 @@
         <v>0.26340000000000002</v>
       </c>
       <c r="L38" s="56" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B39" s="19">
         <v>37</v>
@@ -3594,20 +3554,20 @@
       <c r="C39" s="28">
         <v>6</v>
       </c>
-      <c r="D39" s="63" t="s">
-        <v>251</v>
+      <c r="D39" s="28" t="s">
+        <v>245</v>
       </c>
       <c r="E39" s="28" t="s">
         <v>15</v>
       </c>
       <c r="F39" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G39" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H39" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G39" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H39" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I39" s="38"/>
       <c r="J39" s="59"/>
@@ -3619,7 +3579,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B40" s="19">
         <v>38</v>
@@ -3627,20 +3587,20 @@
       <c r="C40" s="28">
         <v>1</v>
       </c>
-      <c r="D40" s="63" t="s">
+      <c r="D40" s="28" t="s">
         <v>26</v>
       </c>
       <c r="E40" s="28" t="s">
         <v>25</v>
       </c>
       <c r="F40" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G40" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H40" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G40" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H40" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I40" s="35"/>
       <c r="J40" s="58"/>
@@ -3652,7 +3612,7 @@
     </row>
     <row r="41" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B41" s="19">
         <v>39</v>
@@ -3660,20 +3620,20 @@
       <c r="C41" s="28">
         <v>1</v>
       </c>
-      <c r="D41" s="63" t="s">
+      <c r="D41" s="28" t="s">
         <v>12</v>
       </c>
       <c r="E41" s="62" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F41" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G41" s="28" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H41" s="28" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I41" s="35"/>
       <c r="J41" s="59">
@@ -3684,12 +3644,12 @@
         <v>0.18551999999999999</v>
       </c>
       <c r="L41" s="33" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B42" s="19">
         <v>40</v>
@@ -3697,20 +3657,20 @@
       <c r="C42" s="28">
         <v>7</v>
       </c>
-      <c r="D42" s="63" t="s">
-        <v>250</v>
+      <c r="D42" s="28" t="s">
+        <v>244</v>
       </c>
       <c r="E42" s="28" t="s">
         <v>29</v>
       </c>
       <c r="F42" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G42" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H42" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G42" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H42" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I42" s="35"/>
       <c r="J42" s="59"/>
@@ -3722,7 +3682,7 @@
     </row>
     <row r="43" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B43" s="19">
         <v>41</v>
@@ -3730,20 +3690,20 @@
       <c r="C43" s="28">
         <v>7</v>
       </c>
-      <c r="D43" s="63" t="s">
+      <c r="D43" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="E43" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="E43" s="28" t="s">
-        <v>129</v>
-      </c>
       <c r="F43" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G43" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H43" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G43" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H43" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I43" s="38"/>
       <c r="J43" s="59"/>
@@ -3755,7 +3715,7 @@
     </row>
     <row r="44" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B44" s="19">
         <v>42</v>
@@ -3763,20 +3723,20 @@
       <c r="C44" s="28">
         <v>6</v>
       </c>
-      <c r="D44" s="63" t="s">
-        <v>248</v>
+      <c r="D44" s="28" t="s">
+        <v>242</v>
       </c>
       <c r="E44" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F44" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G44" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H44" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G44" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H44" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I44" s="35"/>
       <c r="J44" s="59"/>
@@ -3788,7 +3748,7 @@
     </row>
     <row r="45" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B45" s="19">
         <v>43</v>
@@ -3796,20 +3756,20 @@
       <c r="C45" s="28">
         <v>6</v>
       </c>
-      <c r="D45" s="63" t="s">
-        <v>249</v>
+      <c r="D45" s="28" t="s">
+        <v>243</v>
       </c>
       <c r="E45" s="28" t="s">
         <v>21</v>
       </c>
       <c r="F45" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G45" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H45" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G45" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H45" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I45" s="38"/>
       <c r="J45" s="59"/>
@@ -3821,7 +3781,7 @@
     </row>
     <row r="46" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B46" s="19">
         <v>44</v>
@@ -3829,20 +3789,20 @@
       <c r="C46" s="28">
         <v>7</v>
       </c>
-      <c r="D46" s="63" t="s">
-        <v>174</v>
+      <c r="D46" s="28" t="s">
+        <v>171</v>
       </c>
       <c r="E46" s="28" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F46" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G46" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H46" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G46" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H46" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I46" s="38"/>
       <c r="J46" s="59"/>
@@ -3854,7 +3814,7 @@
     </row>
     <row r="47" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B47" s="19">
         <v>45</v>
@@ -3862,20 +3822,20 @@
       <c r="C47" s="28">
         <v>2</v>
       </c>
-      <c r="D47" s="63" t="s">
-        <v>169</v>
+      <c r="D47" s="28" t="s">
+        <v>166</v>
       </c>
       <c r="E47" s="28" t="s">
         <v>16</v>
       </c>
       <c r="F47" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G47" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H47" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G47" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H47" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I47" s="35"/>
       <c r="J47" s="59"/>
@@ -3887,7 +3847,7 @@
     </row>
     <row r="48" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B48" s="19">
         <v>46</v>
@@ -3895,20 +3855,20 @@
       <c r="C48" s="28">
         <v>2</v>
       </c>
-      <c r="D48" s="63" t="s">
-        <v>171</v>
+      <c r="D48" s="28" t="s">
+        <v>168</v>
       </c>
       <c r="E48" s="28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F48" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G48" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H48" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G48" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H48" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I48" s="38"/>
       <c r="J48" s="59"/>
@@ -3918,42 +3878,27 @@
       </c>
       <c r="L48" s="47"/>
     </row>
-    <row r="49" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A49" s="18" t="s">
-        <v>73</v>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A49" s="19" t="s">
+        <v>69</v>
       </c>
       <c r="B49" s="19">
-        <v>47</v>
-      </c>
-      <c r="C49" s="28">
-        <v>2</v>
-      </c>
-      <c r="D49" s="63" t="s">
-        <v>132</v>
-      </c>
-      <c r="E49" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="F49" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="G49" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H49" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="I49" s="38"/>
+        <v>18</v>
+      </c>
+      <c r="C49" s="66"/>
+      <c r="D49" s="66"/>
+      <c r="E49" s="66"/>
+      <c r="F49" s="66"/>
+      <c r="G49" s="66"/>
+      <c r="H49" s="66"/>
+      <c r="I49" s="37"/>
       <c r="J49" s="58"/>
-      <c r="K49" s="58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L49" s="47"/>
+      <c r="K49" s="58"/>
+      <c r="L49" s="56"/>
     </row>
     <row r="50" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B50" s="19">
         <v>48</v>
@@ -3961,20 +3906,20 @@
       <c r="C50" s="28">
         <v>1</v>
       </c>
-      <c r="D50" s="63" t="s">
+      <c r="D50" s="28" t="s">
         <v>42</v>
       </c>
       <c r="E50" s="28" t="s">
         <v>41</v>
       </c>
       <c r="F50" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G50" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H50" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G50" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H50" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I50" s="35"/>
       <c r="J50" s="58"/>
@@ -3986,28 +3931,28 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B51" s="19">
         <v>49</v>
       </c>
-      <c r="C51" s="74">
+      <c r="C51" s="66">
         <v>0</v>
       </c>
-      <c r="D51" s="74" t="s">
-        <v>165</v>
-      </c>
-      <c r="E51" s="74" t="s">
-        <v>165</v>
-      </c>
-      <c r="F51" s="74" t="s">
-        <v>165</v>
-      </c>
-      <c r="G51" s="74" t="s">
-        <v>176</v>
-      </c>
-      <c r="H51" s="74" t="s">
-        <v>165</v>
+      <c r="D51" s="66" t="s">
+        <v>162</v>
+      </c>
+      <c r="E51" s="66" t="s">
+        <v>162</v>
+      </c>
+      <c r="F51" s="66" t="s">
+        <v>162</v>
+      </c>
+      <c r="G51" s="66" t="s">
+        <v>173</v>
+      </c>
+      <c r="H51" s="66" t="s">
+        <v>162</v>
       </c>
       <c r="I51" s="35"/>
       <c r="J51" s="58"/>
@@ -4019,7 +3964,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B52" s="19">
         <v>50</v>
@@ -4027,20 +3972,20 @@
       <c r="C52" s="28">
         <v>1</v>
       </c>
-      <c r="D52" s="63" t="s">
-        <v>168</v>
+      <c r="D52" s="28" t="s">
+        <v>165</v>
       </c>
       <c r="E52" s="28" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F52" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G52" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H52" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G52" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H52" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I52" s="40"/>
       <c r="J52" s="60"/>
@@ -4052,7 +3997,7 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B53" s="19">
         <v>51</v>
@@ -4060,20 +4005,20 @@
       <c r="C53" s="28">
         <v>1</v>
       </c>
-      <c r="D53" s="63" t="s">
+      <c r="D53" s="28" t="s">
         <v>34</v>
       </c>
       <c r="E53" s="28" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F53" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G53" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H53" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G53" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H53" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I53" s="40"/>
       <c r="J53" s="60"/>
@@ -4085,17 +4030,17 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B54" s="19">
         <v>52</v>
       </c>
-      <c r="C54" s="74"/>
-      <c r="D54" s="74"/>
-      <c r="E54" s="74"/>
-      <c r="F54" s="74"/>
-      <c r="G54" s="74"/>
-      <c r="H54" s="74"/>
+      <c r="C54" s="66"/>
+      <c r="D54" s="66"/>
+      <c r="E54" s="66"/>
+      <c r="F54" s="66"/>
+      <c r="G54" s="66"/>
+      <c r="H54" s="66"/>
       <c r="I54" s="40"/>
       <c r="J54" s="60"/>
       <c r="K54" s="58">
@@ -4106,7 +4051,7 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B55" s="19">
         <v>53</v>
@@ -4114,20 +4059,20 @@
       <c r="C55" s="28">
         <v>1</v>
       </c>
-      <c r="D55" s="63" t="s">
+      <c r="D55" s="28" t="s">
         <v>31</v>
       </c>
       <c r="E55" s="28" t="s">
         <v>30</v>
       </c>
       <c r="F55" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G55" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H55" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G55" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H55" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I55" s="40"/>
       <c r="J55" s="60"/>
@@ -4139,7 +4084,7 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B56" s="19">
         <v>54</v>
@@ -4147,20 +4092,20 @@
       <c r="C56" s="28">
         <v>1</v>
       </c>
-      <c r="D56" s="63" t="s">
+      <c r="D56" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="E56" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="E56" s="28" t="s">
-        <v>82</v>
-      </c>
       <c r="F56" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G56" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H56" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G56" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H56" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I56" s="42"/>
       <c r="J56" s="60"/>
@@ -4172,7 +4117,7 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B57" s="19">
         <v>55</v>
@@ -4180,20 +4125,20 @@
       <c r="C57" s="28">
         <v>1</v>
       </c>
-      <c r="D57" s="63" t="s">
-        <v>136</v>
+      <c r="D57" s="28" t="s">
+        <v>133</v>
       </c>
       <c r="E57" s="28" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F57" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G57" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H57" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G57" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H57" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I57" s="42"/>
       <c r="J57" s="60"/>
@@ -4205,17 +4150,17 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B58" s="19">
         <v>56</v>
       </c>
-      <c r="C58" s="74"/>
-      <c r="D58" s="74"/>
-      <c r="E58" s="74"/>
-      <c r="F58" s="74"/>
-      <c r="G58" s="74"/>
-      <c r="H58" s="74"/>
+      <c r="C58" s="66"/>
+      <c r="D58" s="66"/>
+      <c r="E58" s="66"/>
+      <c r="F58" s="66"/>
+      <c r="G58" s="66"/>
+      <c r="H58" s="66"/>
       <c r="I58" s="42"/>
       <c r="J58" s="60"/>
       <c r="K58" s="58">
@@ -4226,28 +4171,28 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B59" s="19">
         <v>57</v>
       </c>
-      <c r="C59" s="74">
+      <c r="C59" s="66">
         <v>0</v>
       </c>
-      <c r="D59" s="74" t="s">
-        <v>165</v>
-      </c>
-      <c r="E59" s="74" t="s">
-        <v>165</v>
-      </c>
-      <c r="F59" s="74" t="s">
-        <v>165</v>
-      </c>
-      <c r="G59" s="74" t="s">
-        <v>176</v>
-      </c>
-      <c r="H59" s="74" t="s">
-        <v>165</v>
+      <c r="D59" s="66" t="s">
+        <v>162</v>
+      </c>
+      <c r="E59" s="66" t="s">
+        <v>162</v>
+      </c>
+      <c r="F59" s="66" t="s">
+        <v>162</v>
+      </c>
+      <c r="G59" s="66" t="s">
+        <v>173</v>
+      </c>
+      <c r="H59" s="66" t="s">
+        <v>162</v>
       </c>
       <c r="I59" s="42"/>
       <c r="J59" s="60"/>
@@ -4259,7 +4204,7 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B60" s="19">
         <v>58</v>
@@ -4267,20 +4212,20 @@
       <c r="C60" s="28">
         <v>1</v>
       </c>
-      <c r="D60" s="63" t="s">
+      <c r="D60" s="28" t="s">
         <v>23</v>
       </c>
       <c r="E60" s="28" t="s">
         <v>22</v>
       </c>
       <c r="F60" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G60" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H60" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G60" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H60" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I60" s="42"/>
       <c r="J60" s="60"/>
@@ -4292,17 +4237,17 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B61" s="19">
         <v>59</v>
       </c>
-      <c r="C61" s="74"/>
-      <c r="D61" s="74"/>
-      <c r="E61" s="74"/>
-      <c r="F61" s="74"/>
-      <c r="G61" s="74"/>
-      <c r="H61" s="74"/>
+      <c r="C61" s="66"/>
+      <c r="D61" s="66"/>
+      <c r="E61" s="66"/>
+      <c r="F61" s="66"/>
+      <c r="G61" s="66"/>
+      <c r="H61" s="66"/>
       <c r="I61" s="42"/>
       <c r="J61" s="60"/>
       <c r="K61" s="58">
@@ -4313,7 +4258,7 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B62" s="19">
         <v>60</v>
@@ -4321,20 +4266,20 @@
       <c r="C62" s="28">
         <v>1</v>
       </c>
-      <c r="D62" s="63" t="s">
+      <c r="D62" s="28" t="s">
         <v>20</v>
       </c>
       <c r="E62" s="28" t="s">
         <v>19</v>
       </c>
       <c r="F62" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G62" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H62" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G62" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H62" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I62" s="42"/>
       <c r="J62" s="60"/>
@@ -4346,7 +4291,7 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B63" s="19">
         <v>61</v>
@@ -4354,20 +4299,20 @@
       <c r="C63" s="28">
         <v>1</v>
       </c>
-      <c r="D63" s="63" t="s">
+      <c r="D63" s="28" t="s">
         <v>47</v>
       </c>
       <c r="E63" s="28" t="s">
         <v>46</v>
       </c>
       <c r="F63" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G63" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H63" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G63" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H63" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I63" s="42"/>
       <c r="J63" s="60"/>
@@ -4379,7 +4324,7 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B64" s="19">
         <v>62</v>
@@ -4387,20 +4332,20 @@
       <c r="C64" s="28">
         <v>1</v>
       </c>
-      <c r="D64" s="63" t="s">
+      <c r="D64" s="28" t="s">
         <v>40</v>
       </c>
       <c r="E64" s="28" t="s">
         <v>39</v>
       </c>
       <c r="F64" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G64" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H64" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G64" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H64" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I64" s="42"/>
       <c r="J64" s="60"/>
@@ -4412,7 +4357,7 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B65" s="19">
         <v>63</v>
@@ -4420,20 +4365,20 @@
       <c r="C65" s="28">
         <v>1</v>
       </c>
-      <c r="D65" s="63" t="s">
-        <v>154</v>
+      <c r="D65" s="28" t="s">
+        <v>151</v>
       </c>
       <c r="E65" s="28" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F65" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G65" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H65" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G65" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H65" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I65" s="42"/>
       <c r="J65" s="60"/>
@@ -4445,17 +4390,17 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B66" s="19">
         <v>64</v>
       </c>
-      <c r="C66" s="74"/>
-      <c r="D66" s="74"/>
-      <c r="E66" s="75"/>
-      <c r="F66" s="74"/>
-      <c r="G66" s="74"/>
-      <c r="H66" s="74"/>
+      <c r="C66" s="66"/>
+      <c r="D66" s="66"/>
+      <c r="E66" s="67"/>
+      <c r="F66" s="66"/>
+      <c r="G66" s="66"/>
+      <c r="H66" s="66"/>
       <c r="I66" s="40"/>
       <c r="J66" s="60">
         <v>6.2199999999999998E-2</v>
@@ -4465,12 +4410,12 @@
         <v>0</v>
       </c>
       <c r="L66" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B67" s="19">
         <v>65</v>
@@ -4478,20 +4423,20 @@
       <c r="C67" s="28">
         <v>1</v>
       </c>
-      <c r="D67" s="63" t="s">
-        <v>68</v>
+      <c r="D67" s="28" t="s">
+        <v>67</v>
       </c>
       <c r="E67" s="28" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F67" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G67" s="28" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H67" s="28" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="I67" s="40"/>
       <c r="J67" s="60">
@@ -4502,12 +4447,12 @@
         <v>0.91432999999999998</v>
       </c>
       <c r="L67" s="50" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B68" s="19">
         <v>66</v>
@@ -4515,20 +4460,20 @@
       <c r="C68" s="28">
         <v>1</v>
       </c>
-      <c r="D68" s="63" t="s">
+      <c r="D68" s="28" t="s">
         <v>8</v>
       </c>
       <c r="E68" s="28" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F68" s="28" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="G68" s="28" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H68" s="28" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="I68" s="40"/>
       <c r="J68" s="60">
@@ -4539,12 +4484,12 @@
         <v>0.53656000000000004</v>
       </c>
       <c r="L68" s="50" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B69" s="19">
         <v>67</v>
@@ -4552,20 +4497,20 @@
       <c r="C69" s="28">
         <v>1</v>
       </c>
-      <c r="D69" s="63" t="s">
+      <c r="D69" s="28" t="s">
         <v>48</v>
       </c>
       <c r="E69" s="28" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F69" s="28" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G69" s="28" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H69" s="28" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I69" s="40"/>
       <c r="J69" s="60">
@@ -4576,22 +4521,22 @@
         <v>0.65</v>
       </c>
       <c r="L69" s="50" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B70" s="19">
         <v>68</v>
       </c>
-      <c r="C70" s="74"/>
-      <c r="D70" s="74"/>
-      <c r="E70" s="74"/>
-      <c r="F70" s="74"/>
-      <c r="G70" s="74"/>
-      <c r="H70" s="74"/>
+      <c r="C70" s="66"/>
+      <c r="D70" s="66"/>
+      <c r="E70" s="66"/>
+      <c r="F70" s="66"/>
+      <c r="G70" s="66"/>
+      <c r="H70" s="66"/>
       <c r="I70" s="40"/>
       <c r="J70" s="60"/>
       <c r="K70" s="58">
@@ -4601,7 +4546,7 @@
     </row>
     <row r="71" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="51" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B71" s="19">
         <v>69</v>
@@ -4609,20 +4554,20 @@
       <c r="C71" s="28">
         <v>1</v>
       </c>
-      <c r="D71" s="63" t="s">
-        <v>139</v>
+      <c r="D71" s="28" t="s">
+        <v>136</v>
       </c>
       <c r="E71" s="28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F71" s="28" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G71" s="28" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H71" s="28" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I71" s="40"/>
       <c r="J71" s="60">
@@ -4633,12 +4578,12 @@
         <v>0.42686000000000002</v>
       </c>
       <c r="L71" s="50" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B72" s="19">
         <v>70</v>
@@ -4646,20 +4591,20 @@
       <c r="C72" s="28">
         <v>1</v>
       </c>
-      <c r="D72" s="63" t="s">
-        <v>142</v>
+      <c r="D72" s="28" t="s">
+        <v>139</v>
       </c>
       <c r="E72" s="28" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F72" s="28" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G72" s="28" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H72" s="28" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I72" s="43"/>
       <c r="J72" s="59">
@@ -4670,12 +4615,12 @@
         <v>1.2505999999999999</v>
       </c>
       <c r="L72" s="46" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B73" s="19">
         <v>71</v>
@@ -4683,20 +4628,20 @@
       <c r="C73" s="28">
         <v>0</v>
       </c>
-      <c r="D73" s="63" t="s">
+      <c r="D73" s="28" t="s">
         <v>6</v>
       </c>
       <c r="E73" s="28" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F73" s="28" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G73" s="28" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H73" s="28" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I73" s="40"/>
       <c r="J73" s="60"/>
@@ -4705,12 +4650,12 @@
         <v>0</v>
       </c>
       <c r="L73" s="57" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B74" s="19">
         <v>72</v>
@@ -4718,17 +4663,17 @@
       <c r="C74" s="28">
         <v>2</v>
       </c>
-      <c r="D74" s="63" t="s">
+      <c r="D74" s="28" t="s">
         <v>44</v>
       </c>
       <c r="E74" s="28" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F74" s="28">
         <v>7414</v>
       </c>
       <c r="G74" s="28" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H74" s="28" t="s">
         <v>45</v>
@@ -4742,12 +4687,12 @@
         <v>0.54127999999999998</v>
       </c>
       <c r="L74" s="50" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B75" s="19">
         <v>73</v>
@@ -4755,20 +4700,20 @@
       <c r="C75" s="28">
         <v>1</v>
       </c>
-      <c r="D75" s="63" t="s">
-        <v>62</v>
+      <c r="D75" s="28" t="s">
+        <v>61</v>
       </c>
       <c r="E75" s="28" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F75" s="28" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G75" s="28" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H75" s="28" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I75" s="41"/>
       <c r="J75" s="60">
@@ -4779,12 +4724,12 @@
         <v>1.0848</v>
       </c>
       <c r="L75" s="50" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B76" s="19">
         <v>74</v>
@@ -4792,20 +4737,20 @@
       <c r="C76" s="28">
         <v>1</v>
       </c>
-      <c r="D76" s="63" t="s">
-        <v>58</v>
+      <c r="D76" s="28" t="s">
+        <v>57</v>
       </c>
       <c r="E76" s="28" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F76" s="28" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G76" s="28" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="H76" s="28" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I76" s="40"/>
       <c r="J76" s="60">
@@ -4816,12 +4761,12 @@
         <v>0.75968000000000002</v>
       </c>
       <c r="L76" s="50" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B77" s="19">
         <v>75</v>
@@ -4829,7 +4774,7 @@
       <c r="C77" s="28">
         <v>1</v>
       </c>
-      <c r="D77" s="63" t="s">
+      <c r="D77" s="28" t="s">
         <v>10</v>
       </c>
       <c r="E77" s="28" t="s">
@@ -4839,7 +4784,7 @@
         <v>9</v>
       </c>
       <c r="G77" s="28" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="H77" s="28"/>
       <c r="I77" s="40"/>
@@ -4851,12 +4796,12 @@
         <v>1.02728</v>
       </c>
       <c r="L77" s="50" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B78" s="19">
         <v>76</v>
@@ -4864,20 +4809,20 @@
       <c r="C78" s="28">
         <v>1</v>
       </c>
-      <c r="D78" s="63" t="s">
+      <c r="D78" s="28" t="s">
         <v>11</v>
       </c>
       <c r="E78" s="28" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F78" s="28" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G78" s="28" t="s">
         <v>50</v>
       </c>
       <c r="H78" s="28" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="I78" s="40"/>
       <c r="J78" s="60">
@@ -4888,22 +4833,22 @@
         <v>0.28182000000000001</v>
       </c>
       <c r="L78" s="50" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B79" s="19">
         <v>77</v>
       </c>
-      <c r="C79" s="74"/>
-      <c r="D79" s="74"/>
-      <c r="E79" s="74"/>
-      <c r="F79" s="74"/>
-      <c r="G79" s="74"/>
-      <c r="H79" s="74"/>
+      <c r="C79" s="66"/>
+      <c r="D79" s="66"/>
+      <c r="E79" s="66"/>
+      <c r="F79" s="66"/>
+      <c r="G79" s="66"/>
+      <c r="H79" s="66"/>
       <c r="I79" s="40"/>
       <c r="J79" s="60">
         <v>0.86136000000000001</v>
@@ -4913,12 +4858,12 @@
         <v>0</v>
       </c>
       <c r="L79" s="50" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B80" s="19">
         <v>78</v>
@@ -4926,20 +4871,20 @@
       <c r="C80" s="28">
         <v>1</v>
       </c>
-      <c r="D80" s="63" t="s">
+      <c r="D80" s="28" t="s">
         <v>18</v>
       </c>
       <c r="E80" s="28" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F80" s="28" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G80" s="28" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H80" s="28" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I80" s="40"/>
       <c r="J80" s="60">
@@ -4950,12 +4895,12 @@
         <v>0.57067999999999997</v>
       </c>
       <c r="L80" s="50" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B81" s="19">
         <v>79</v>
@@ -4963,20 +4908,20 @@
       <c r="C81" s="28">
         <v>1</v>
       </c>
-      <c r="D81" s="65" t="s">
-        <v>159</v>
+      <c r="D81" s="64" t="s">
+        <v>156</v>
       </c>
       <c r="E81" s="44" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F81" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G81" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H81" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G81" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H81" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I81" s="40"/>
       <c r="J81" s="60"/>
@@ -4987,7 +4932,7 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B82" s="19">
         <v>80</v>
@@ -4995,11 +4940,11 @@
       <c r="C82" s="28">
         <v>0</v>
       </c>
-      <c r="D82" s="65" t="s">
-        <v>160</v>
+      <c r="D82" s="64" t="s">
+        <v>157</v>
       </c>
       <c r="E82" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F82" s="28" t="s">
         <v>49</v>
@@ -5020,7 +4965,7 @@
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B83" s="19">
         <v>81</v>
@@ -5028,20 +4973,20 @@
       <c r="C83" s="28">
         <v>1</v>
       </c>
-      <c r="D83" s="63" t="s">
+      <c r="D83" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="E83" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="F83" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G83" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="E83" s="28" t="s">
-        <v>170</v>
-      </c>
-      <c r="F83" s="28" t="s">
+      <c r="H83" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G83" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H83" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I83" s="40"/>
       <c r="J83" s="60"/>
@@ -5055,11 +5000,11 @@
       <c r="G84" s="45"/>
       <c r="J84" s="61">
         <f>SUM(J7:J83)</f>
-        <v>13.288069999999996</v>
+        <v>13.179349999999998</v>
       </c>
       <c r="K84" s="61">
         <f>SUM(K7:K83)</f>
-        <v>12.826489999999998</v>
+        <v>12.717769999999998</v>
       </c>
     </row>
   </sheetData>
@@ -5086,24 +5031,23 @@
     <hyperlink ref="L28" r:id="rId11" xr:uid="{518A6692-3A50-F942-B48D-CC4356762EAD}"/>
     <hyperlink ref="L22" r:id="rId12" xr:uid="{A1379108-F295-EE45-B6ED-5162031D55EB}"/>
     <hyperlink ref="L7" r:id="rId13" xr:uid="{5948B746-AAC4-5740-AB8C-E151299C82FE}"/>
-    <hyperlink ref="L21" r:id="rId14" xr:uid="{7F2AFDE5-1B48-DB4E-A5DC-FF059C0FC2B5}"/>
-    <hyperlink ref="L24" r:id="rId15" xr:uid="{646B658D-AE56-44EA-A58F-40CDBDEF2D0C}"/>
-    <hyperlink ref="L26" r:id="rId16" xr:uid="{47FDBB7E-44E8-4353-9597-0562E7BF59F5}"/>
-    <hyperlink ref="L27" r:id="rId17" xr:uid="{8736A480-3930-45F7-AECD-F285FFC9909F}"/>
-    <hyperlink ref="L30" r:id="rId18" xr:uid="{F9FA5EE5-1B77-4F3B-8F3F-3842AA6F0BAA}"/>
-    <hyperlink ref="L33" r:id="rId19" xr:uid="{AB84C394-095B-406A-966B-81DF3D2E2812}"/>
-    <hyperlink ref="L31" r:id="rId20" xr:uid="{C8A6F598-6C7B-4E81-A0E7-EBB0B449E508}"/>
-    <hyperlink ref="L32" r:id="rId21" xr:uid="{51DB6C5F-D3B9-4DE7-B2D3-FC15FA2E815B}"/>
-    <hyperlink ref="L34" r:id="rId22" xr:uid="{1E8D4B86-2BB1-4BC4-B74E-EFE1D1B71B87}"/>
-    <hyperlink ref="L37" r:id="rId23" xr:uid="{E3611F41-7D12-4600-84CB-E5DA78E4D275}"/>
-    <hyperlink ref="L38" r:id="rId24" xr:uid="{F8FD3DE4-2053-469C-A880-F854815B0BBC}"/>
-    <hyperlink ref="L67" r:id="rId25" xr:uid="{5E58DFC9-92C6-487D-82FB-789F079E9373}"/>
-    <hyperlink ref="L68" r:id="rId26" xr:uid="{9D884BB0-E9D5-416B-B348-A3CCA307ED67}"/>
-    <hyperlink ref="L73" r:id="rId27" xr:uid="{4AD4981F-0482-460C-B12B-D6E5A82469EE}"/>
-    <hyperlink ref="L78" r:id="rId28" xr:uid="{168580DB-C131-4BC7-9E3D-A9AEB4A7EE65}"/>
+    <hyperlink ref="L24" r:id="rId14" xr:uid="{646B658D-AE56-44EA-A58F-40CDBDEF2D0C}"/>
+    <hyperlink ref="L26" r:id="rId15" xr:uid="{47FDBB7E-44E8-4353-9597-0562E7BF59F5}"/>
+    <hyperlink ref="L27" r:id="rId16" xr:uid="{8736A480-3930-45F7-AECD-F285FFC9909F}"/>
+    <hyperlink ref="L30" r:id="rId17" xr:uid="{F9FA5EE5-1B77-4F3B-8F3F-3842AA6F0BAA}"/>
+    <hyperlink ref="L33" r:id="rId18" xr:uid="{AB84C394-095B-406A-966B-81DF3D2E2812}"/>
+    <hyperlink ref="L31" r:id="rId19" xr:uid="{C8A6F598-6C7B-4E81-A0E7-EBB0B449E508}"/>
+    <hyperlink ref="L32" r:id="rId20" xr:uid="{51DB6C5F-D3B9-4DE7-B2D3-FC15FA2E815B}"/>
+    <hyperlink ref="L34" r:id="rId21" xr:uid="{1E8D4B86-2BB1-4BC4-B74E-EFE1D1B71B87}"/>
+    <hyperlink ref="L37" r:id="rId22" xr:uid="{E3611F41-7D12-4600-84CB-E5DA78E4D275}"/>
+    <hyperlink ref="L38" r:id="rId23" xr:uid="{F8FD3DE4-2053-469C-A880-F854815B0BBC}"/>
+    <hyperlink ref="L67" r:id="rId24" xr:uid="{5E58DFC9-92C6-487D-82FB-789F079E9373}"/>
+    <hyperlink ref="L68" r:id="rId25" xr:uid="{9D884BB0-E9D5-416B-B348-A3CCA307ED67}"/>
+    <hyperlink ref="L73" r:id="rId26" xr:uid="{4AD4981F-0482-460C-B12B-D6E5A82469EE}"/>
+    <hyperlink ref="L78" r:id="rId27" xr:uid="{168580DB-C131-4BC7-9E3D-A9AEB4A7EE65}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
 
@@ -5111,10 +5055,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="1">
+    <sheetView topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="1">
       <selection activeCell="C4" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
@@ -5127,7 +5071,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1"/>
     </row>
@@ -5137,38 +5081,38 @@
     </row>
     <row r="3" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D3" s="53" t="s">
         <v>78</v>
-      </c>
-      <c r="D3" s="53" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="68" t="s">
-        <v>157</v>
-      </c>
-      <c r="B4" s="69">
-        <v>45020</v>
-      </c>
-      <c r="C4" s="70" t="s">
-        <v>156</v>
+        <v>154</v>
+      </c>
+      <c r="B4" s="70">
+        <v>45246</v>
+      </c>
+      <c r="C4" s="72" t="s">
+        <v>153</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="204" x14ac:dyDescent="0.2">
-      <c r="A5" s="71"/>
-      <c r="B5" s="72"/>
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="229.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="69"/>
+      <c r="B5" s="71"/>
       <c r="C5" s="73"/>
       <c r="D5" s="34" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Actualizacion BOM MK1 RP2040 y cambios menores
Se agranda los agujeros laterales del rotary.
Intercambio de posición de las vías del pedal.
Acortamiento de la peninsula.
</commit_message>
<xml_diff>
--- a/02.Hardware/MK1-RP2040/01.EDCPSU/BOM/EDCPSU_MK1_RP2040_BOM-SETI.xlsx
+++ b/02.Hardware/MK1-RP2040/01.EDCPSU/BOM/EDCPSU_MK1_RP2040_BOM-SETI.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Team Dropbox\JRODRIGUEZ\Repositorios\11.MK1\02.Hardware\MK1-RP2040\01.EDCPSU\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC428E32-E1F1-48B9-9BF5-0B7C78098F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9A3C8F-3C02-4429-8A1B-4D619D28013D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19215" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="18900" yWindow="0" windowWidth="10005" windowHeight="15585" activeTab="1" xr2:uid="{CDEA638F-CF3E-43EC-96DC-54CE86003FCC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CDEA638F-CF3E-43EC-96DC-54CE86003FCC}"/>
   </bookViews>
   <sheets>
     <sheet name="EDCPSUMK1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="249">
   <si>
     <t>Qty</t>
   </si>
@@ -196,9 +196,6 @@
     <t>DO-214AB</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
     <t>Display</t>
   </si>
   <si>
@@ -433,12 +430,6 @@
     <t>150K</t>
   </si>
   <si>
-    <t>R38, R63</t>
-  </si>
-  <si>
-    <t>27R</t>
-  </si>
-  <si>
     <t>27K</t>
   </si>
   <si>
@@ -733,15 +724,6 @@
     <t>TVS 18V 400W Unidirectional</t>
   </si>
   <si>
-    <t>https://www.digikey.es/en/products/detail/littelfuse-inc/SMAJ24A/762288</t>
-  </si>
-  <si>
-    <t>ESD Suppressors / TVS Diodes 24volts 5uA 10.3 Amps UNI-Dir</t>
-  </si>
-  <si>
-    <t>SMAJ24A</t>
-  </si>
-  <si>
     <t>COST (500pcs)</t>
   </si>
   <si>
@@ -791,6 +773,12 @@
   </si>
   <si>
     <t>R1,R32, R39, R40, R42, R66</t>
+  </si>
+  <si>
+    <t>BOM VERSION v1</t>
+  </si>
+  <si>
+    <t>MK1-RP2040</t>
   </si>
   <si>
     <t>Modificaciones frente a la v4 de la MK2-RP2040:
@@ -808,13 +796,9 @@
 Se elimina la posicion 59, part R62
 Se elimina la posicion 64, part RSENSE
 Se elimina la posicion 68, part U10
-Se elimina la posicion 77, part U9</t>
-  </si>
-  <si>
-    <t>BOM VERSION v1</t>
-  </si>
-  <si>
-    <t>MK1-RP2040</t>
+Se elimina la posicion 77, part U9
+Se elimina la posicion 16, part D1
+Se elimina la posicion 47, part R38 y R63</t>
   </si>
 </sst>
 </file>
@@ -1775,7 +1759,7 @@
     <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1943,44 +1927,38 @@
     <xf numFmtId="0" fontId="47" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="47" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="85">
@@ -2395,17 +2373,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="1">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="8" customWidth="1"/>
     <col min="2" max="2" width="4" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" style="66" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.140625" style="5" bestFit="1" customWidth="1"/>
@@ -2418,7 +2398,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="D1" s="3" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="J1"/>
     </row>
@@ -2429,26 +2409,25 @@
       <c r="J2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D3" s="67"/>
+      <c r="D3" s="65"/>
       <c r="J3"/>
     </row>
     <row r="4" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D4" s="2" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="J4"/>
     </row>
     <row r="5" spans="1:12" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="D5" s="7"/>
       <c r="G5" s="1"/>
       <c r="J5"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>0</v>
@@ -2469,21 +2448,21 @@
         <v>5</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" s="19">
         <v>2</v>
@@ -2491,20 +2470,20 @@
       <c r="C7" s="28">
         <v>1</v>
       </c>
-      <c r="D7" s="63" t="s">
-        <v>57</v>
+      <c r="D7" s="28" t="s">
+        <v>56</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I7" s="36"/>
       <c r="J7" s="58">
@@ -2515,12 +2494,12 @@
         <v>0.48</v>
       </c>
       <c r="L7" s="46" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="19">
         <v>3</v>
@@ -2528,17 +2507,17 @@
       <c r="C8" s="28">
         <v>3</v>
       </c>
-      <c r="D8" s="63" t="s">
+      <c r="D8" s="28" t="s">
         <v>35</v>
       </c>
       <c r="E8" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="F8" s="28" t="s">
-        <v>85</v>
-      </c>
       <c r="G8" s="28" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H8" s="28" t="s">
         <v>14</v>
@@ -2552,12 +2531,12 @@
         <v>0.31794</v>
       </c>
       <c r="L8" s="33" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" s="19">
         <v>4</v>
@@ -2565,17 +2544,17 @@
       <c r="C9" s="28">
         <v>0</v>
       </c>
-      <c r="D9" s="63" t="s">
-        <v>102</v>
+      <c r="D9" s="28" t="s">
+        <v>101</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F9" s="28" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H9" s="28" t="s">
         <v>14</v>
@@ -2590,7 +2569,7 @@
     </row>
     <row r="10" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B10" s="19">
         <v>5</v>
@@ -2598,17 +2577,17 @@
       <c r="C10" s="28">
         <v>32</v>
       </c>
-      <c r="D10" s="64" t="s">
-        <v>245</v>
+      <c r="D10" s="63" t="s">
+        <v>239</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F10" s="28" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H10" s="28" t="s">
         <v>14</v>
@@ -2623,7 +2602,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" s="19">
         <v>6</v>
@@ -2631,17 +2610,17 @@
       <c r="C11" s="28">
         <v>4</v>
       </c>
-      <c r="D11" s="63" t="s">
+      <c r="D11" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="62" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="62" t="s">
-        <v>88</v>
-      </c>
       <c r="F11" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H11" s="28" t="s">
         <v>14</v>
@@ -2655,12 +2634,12 @@
         <v>0.27688000000000001</v>
       </c>
       <c r="L11" s="33" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12" s="19">
         <v>7</v>
@@ -2668,17 +2647,17 @@
       <c r="C12" s="28">
         <v>2</v>
       </c>
-      <c r="D12" s="63" t="s">
-        <v>89</v>
+      <c r="D12" s="28" t="s">
+        <v>88</v>
       </c>
       <c r="E12" s="62" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F12" s="28" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H12" s="28" t="s">
         <v>14</v>
@@ -2692,12 +2671,12 @@
         <v>0.11260000000000001</v>
       </c>
       <c r="L12" s="33" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" s="19">
         <v>8</v>
@@ -2705,17 +2684,17 @@
       <c r="C13" s="28">
         <v>1</v>
       </c>
-      <c r="D13" s="63" t="s">
+      <c r="D13" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13" s="28" t="s">
         <v>90</v>
-      </c>
-      <c r="E13" s="28" t="s">
-        <v>91</v>
       </c>
       <c r="F13" s="28" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H13" s="28" t="s">
         <v>14</v>
@@ -2730,7 +2709,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B14" s="19">
         <v>9</v>
@@ -2738,17 +2717,17 @@
       <c r="C14" s="28">
         <v>1</v>
       </c>
-      <c r="D14" s="63" t="s">
+      <c r="D14" s="28" t="s">
         <v>24</v>
       </c>
       <c r="E14" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F14" s="28" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H14" s="28" t="s">
         <v>14</v>
@@ -2763,7 +2742,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B15" s="19">
         <v>10</v>
@@ -2771,17 +2750,17 @@
       <c r="C15" s="28">
         <v>1</v>
       </c>
-      <c r="D15" s="63" t="s">
+      <c r="D15" s="28" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F15" s="28" t="s">
         <v>13</v>
       </c>
       <c r="G15" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H15" s="28" t="s">
         <v>14</v>
@@ -2796,7 +2775,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" s="19">
         <v>11</v>
@@ -2804,17 +2783,17 @@
       <c r="C16" s="28">
         <v>4</v>
       </c>
-      <c r="D16" s="63" t="s">
+      <c r="D16" s="28" t="s">
         <v>27</v>
       </c>
       <c r="E16" s="62" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G16" s="28" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H16" s="28" t="s">
         <v>14</v>
@@ -2828,12 +2807,12 @@
         <v>0.49447999999999998</v>
       </c>
       <c r="L16" s="33" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B17" s="19">
         <v>12</v>
@@ -2841,17 +2820,17 @@
       <c r="C17" s="28">
         <v>0</v>
       </c>
-      <c r="D17" s="63" t="s">
+      <c r="D17" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" s="28" t="s">
         <v>94</v>
-      </c>
-      <c r="E17" s="28" t="s">
-        <v>95</v>
       </c>
       <c r="F17" s="28" t="s">
         <v>13</v>
       </c>
       <c r="G17" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H17" s="28" t="s">
         <v>14</v>
@@ -2866,7 +2845,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B18" s="19">
         <v>13</v>
@@ -2874,17 +2853,17 @@
       <c r="C18" s="28">
         <v>2</v>
       </c>
-      <c r="D18" s="63" t="s">
+      <c r="D18" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18" s="28" t="s">
         <v>96</v>
-      </c>
-      <c r="E18" s="28" t="s">
-        <v>97</v>
       </c>
       <c r="F18" s="28" t="s">
         <v>13</v>
       </c>
       <c r="G18" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H18" s="28" t="s">
         <v>14</v>
@@ -2899,7 +2878,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19" s="19">
         <v>14</v>
@@ -2907,17 +2886,17 @@
       <c r="C19" s="28">
         <v>2</v>
       </c>
-      <c r="D19" s="63" t="s">
+      <c r="D19" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" s="62" t="s">
         <v>98</v>
-      </c>
-      <c r="E19" s="62" t="s">
-        <v>99</v>
       </c>
       <c r="F19" s="28" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H19" s="28" t="s">
         <v>14</v>
@@ -2931,12 +2910,12 @@
         <v>8.5519999999999999E-2</v>
       </c>
       <c r="L19" s="33" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B20" s="19">
         <v>15</v>
@@ -2944,17 +2923,17 @@
       <c r="C20" s="28">
         <v>7</v>
       </c>
-      <c r="D20" s="63" t="s">
-        <v>246</v>
+      <c r="D20" s="28" t="s">
+        <v>240</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F20" s="28" t="s">
         <v>13</v>
       </c>
       <c r="G20" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H20" s="28" t="s">
         <v>14</v>
@@ -2968,45 +2947,26 @@
       <c r="L20" s="33"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="18" t="s">
-        <v>73</v>
+      <c r="A21" s="19" t="s">
+        <v>69</v>
       </c>
       <c r="B21" s="19">
-        <v>16</v>
-      </c>
-      <c r="C21" s="28">
-        <v>1</v>
-      </c>
-      <c r="D21" s="63" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>234</v>
-      </c>
-      <c r="F21" s="28" t="s">
-        <v>234</v>
-      </c>
-      <c r="G21" s="28" t="s">
-        <v>227</v>
-      </c>
-      <c r="H21" s="28" t="s">
-        <v>233</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C21" s="66"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="66"/>
+      <c r="G21" s="66"/>
+      <c r="H21" s="66"/>
       <c r="I21" s="37"/>
-      <c r="J21" s="58">
-        <v>0.10872</v>
-      </c>
-      <c r="K21" s="58">
-        <f t="shared" si="0"/>
-        <v>0.10872</v>
-      </c>
-      <c r="L21" s="56" t="s">
-        <v>232</v>
-      </c>
+      <c r="J21" s="58"/>
+      <c r="K21" s="58"/>
+      <c r="L21" s="56"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B22" s="19">
         <v>17</v>
@@ -3014,8 +2974,8 @@
       <c r="C22" s="28">
         <v>2</v>
       </c>
-      <c r="D22" s="63" t="s">
-        <v>161</v>
+      <c r="D22" s="28" t="s">
+        <v>158</v>
       </c>
       <c r="E22" s="28" t="s">
         <v>49</v>
@@ -3038,22 +2998,22 @@
         <v>0.22900000000000001</v>
       </c>
       <c r="L22" s="46" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B23" s="19">
         <v>18</v>
       </c>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="74"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="66"/>
       <c r="I23" s="37"/>
       <c r="J23" s="58"/>
       <c r="K23" s="58"/>
@@ -3061,7 +3021,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B24" s="19">
         <v>19</v>
@@ -3069,20 +3029,20 @@
       <c r="C24" s="28">
         <v>1</v>
       </c>
-      <c r="D24" s="63" t="s">
+      <c r="D24" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="E24" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="E24" s="28" t="s">
+      <c r="F24" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="H24" s="28" t="s">
         <v>107</v>
-      </c>
-      <c r="F24" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="G24" s="28" t="s">
-        <v>227</v>
-      </c>
-      <c r="H24" s="28" t="s">
-        <v>108</v>
       </c>
       <c r="I24" s="37"/>
       <c r="J24" s="58">
@@ -3093,12 +3053,12 @@
         <v>0.1181</v>
       </c>
       <c r="L24" s="56" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B25" s="19">
         <v>20</v>
@@ -3106,14 +3066,14 @@
       <c r="C25" s="28">
         <v>0</v>
       </c>
-      <c r="D25" s="63" t="s">
-        <v>83</v>
+      <c r="D25" s="28" t="s">
+        <v>82</v>
       </c>
       <c r="E25" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F25" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G25" s="28" t="s">
         <v>52</v>
@@ -3129,7 +3089,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B26" s="19">
         <v>21</v>
@@ -3137,20 +3097,20 @@
       <c r="C26" s="28">
         <v>1</v>
       </c>
-      <c r="D26" s="63" t="s">
-        <v>66</v>
+      <c r="D26" s="28" t="s">
+        <v>65</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F26" s="28" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="G26" s="28" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="H26" s="28" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="I26" s="37"/>
       <c r="J26" s="58">
@@ -3161,12 +3121,12 @@
         <v>0.12508</v>
       </c>
       <c r="L26" s="46" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B27" s="19">
         <v>22</v>
@@ -3174,20 +3134,20 @@
       <c r="C27" s="28">
         <v>1</v>
       </c>
-      <c r="D27" s="63" t="s">
-        <v>110</v>
+      <c r="D27" s="28" t="s">
+        <v>109</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F27" s="28" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G27" s="28" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H27" s="28" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="I27" s="38"/>
       <c r="J27" s="58">
@@ -3198,22 +3158,22 @@
         <v>8.6999999999999994E-2</v>
       </c>
       <c r="L27" s="46" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B28" s="19">
         <v>25</v>
       </c>
-      <c r="C28" s="74"/>
-      <c r="D28" s="74"/>
-      <c r="E28" s="74"/>
-      <c r="F28" s="74"/>
-      <c r="G28" s="74"/>
-      <c r="H28" s="74"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="66"/>
       <c r="I28" s="38"/>
       <c r="J28" s="58">
         <v>1.0803</v>
@@ -3223,12 +3183,12 @@
         <v>0</v>
       </c>
       <c r="L28" s="46" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B29" s="19">
         <v>26</v>
@@ -3236,17 +3196,17 @@
       <c r="C29" s="28">
         <v>1</v>
       </c>
-      <c r="D29" s="63" t="s">
-        <v>56</v>
+      <c r="D29" s="28" t="s">
+        <v>55</v>
       </c>
       <c r="E29" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="F29" s="28" t="s">
-        <v>55</v>
-      </c>
       <c r="G29" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H29" s="28"/>
       <c r="I29" s="38"/>
@@ -3259,7 +3219,7 @@
     </row>
     <row r="30" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B30" s="19">
         <v>27</v>
@@ -3267,20 +3227,20 @@
       <c r="C30" s="28">
         <v>1</v>
       </c>
-      <c r="D30" s="63" t="s">
+      <c r="D30" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="E30" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="E30" s="28" t="s">
+      <c r="F30" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="H30" s="28" t="s">
         <v>112</v>
-      </c>
-      <c r="F30" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="G30" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="H30" s="28" t="s">
-        <v>113</v>
       </c>
       <c r="I30" s="38"/>
       <c r="J30" s="58">
@@ -3291,12 +3251,12 @@
         <v>0.64117000000000002</v>
       </c>
       <c r="L30" s="56" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B31" s="19">
         <v>29</v>
@@ -3304,20 +3264,20 @@
       <c r="C31" s="28">
         <v>1</v>
       </c>
-      <c r="D31" s="63" t="s">
+      <c r="D31" s="28" t="s">
         <v>43</v>
       </c>
       <c r="E31" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F31" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="G31" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="F31" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="G31" s="28" t="s">
+      <c r="H31" s="28" t="s">
         <v>115</v>
-      </c>
-      <c r="H31" s="28" t="s">
-        <v>116</v>
       </c>
       <c r="I31" s="38"/>
       <c r="J31" s="59">
@@ -3328,12 +3288,12 @@
         <v>0.12452000000000001</v>
       </c>
       <c r="L31" s="56" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B32" s="19">
         <v>30</v>
@@ -3341,14 +3301,14 @@
       <c r="C32" s="28">
         <v>1</v>
       </c>
-      <c r="D32" s="63" t="s">
+      <c r="D32" s="28" t="s">
         <v>38</v>
       </c>
       <c r="E32" s="28" t="s">
         <v>36</v>
       </c>
       <c r="F32" s="28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G32" s="28" t="s">
         <v>37</v>
@@ -3363,12 +3323,12 @@
         <v>0.72116000000000002</v>
       </c>
       <c r="L32" s="46" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B33" s="19">
         <v>31</v>
@@ -3376,20 +3336,20 @@
       <c r="C33" s="28">
         <v>5</v>
       </c>
-      <c r="D33" s="63" t="s">
-        <v>64</v>
+      <c r="D33" s="28" t="s">
+        <v>63</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F33" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G33" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H33" s="28" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I33" s="38"/>
       <c r="J33" s="59">
@@ -3400,12 +3360,12 @@
         <v>0.11499999999999999</v>
       </c>
       <c r="L33" s="57" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B34" s="19">
         <v>32</v>
@@ -3413,20 +3373,20 @@
       <c r="C34" s="28">
         <v>1</v>
       </c>
-      <c r="D34" s="63" t="s">
+      <c r="D34" s="28" t="s">
         <v>7</v>
       </c>
       <c r="E34" s="28" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F34" s="28" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="G34" s="28" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="H34" s="28" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="I34" s="38"/>
       <c r="J34" s="59">
@@ -3437,12 +3397,12 @@
         <v>3.4189999999999998E-2</v>
       </c>
       <c r="L34" s="46" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B35" s="19">
         <v>33</v>
@@ -3450,20 +3410,20 @@
       <c r="C35" s="28">
         <v>0</v>
       </c>
-      <c r="D35" s="63" t="s">
+      <c r="D35" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E35" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="E35" s="28" t="s">
+      <c r="F35" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="G35" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="F35" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="G35" s="28" t="s">
+      <c r="H35" s="28" t="s">
         <v>120</v>
-      </c>
-      <c r="H35" s="28" t="s">
-        <v>121</v>
       </c>
       <c r="I35" s="39"/>
       <c r="J35" s="58"/>
@@ -3475,7 +3435,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B36" s="19">
         <v>34</v>
@@ -3483,20 +3443,20 @@
       <c r="C36" s="28">
         <v>1</v>
       </c>
-      <c r="D36" s="63" t="s">
+      <c r="D36" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E36" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="F36" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G36" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="H36" s="28" t="s">
         <v>60</v>
-      </c>
-      <c r="E36" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="F36" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="G36" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="H36" s="28" t="s">
-        <v>61</v>
       </c>
       <c r="I36" s="35"/>
       <c r="J36" s="58">
@@ -3507,12 +3467,12 @@
         <v>0.1341</v>
       </c>
       <c r="L36" s="46" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B37" s="19">
         <v>35</v>
@@ -3520,20 +3480,20 @@
       <c r="C37" s="28">
         <v>1</v>
       </c>
-      <c r="D37" s="63" t="s">
+      <c r="D37" s="28" t="s">
         <v>28</v>
       </c>
       <c r="E37" s="28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F37" s="28" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G37" s="28" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="H37" s="49" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="I37" s="38"/>
       <c r="J37" s="59">
@@ -3544,12 +3504,12 @@
         <v>0.12822</v>
       </c>
       <c r="L37" s="57" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B38" s="19">
         <v>36</v>
@@ -3557,20 +3517,20 @@
       <c r="C38" s="28">
         <v>3</v>
       </c>
-      <c r="D38" s="63" t="s">
-        <v>247</v>
+      <c r="D38" s="28" t="s">
+        <v>241</v>
       </c>
       <c r="E38" s="28" t="s">
         <v>32</v>
       </c>
       <c r="F38" s="28" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G38" s="28" t="s">
         <v>33</v>
       </c>
       <c r="H38" s="28" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="I38" s="38"/>
       <c r="J38" s="59">
@@ -3581,12 +3541,12 @@
         <v>0.26340000000000002</v>
       </c>
       <c r="L38" s="56" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B39" s="19">
         <v>37</v>
@@ -3594,20 +3554,20 @@
       <c r="C39" s="28">
         <v>6</v>
       </c>
-      <c r="D39" s="63" t="s">
-        <v>251</v>
+      <c r="D39" s="28" t="s">
+        <v>245</v>
       </c>
       <c r="E39" s="28" t="s">
         <v>15</v>
       </c>
       <c r="F39" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G39" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H39" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G39" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H39" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I39" s="38"/>
       <c r="J39" s="59"/>
@@ -3619,7 +3579,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B40" s="19">
         <v>38</v>
@@ -3627,20 +3587,20 @@
       <c r="C40" s="28">
         <v>1</v>
       </c>
-      <c r="D40" s="63" t="s">
+      <c r="D40" s="28" t="s">
         <v>26</v>
       </c>
       <c r="E40" s="28" t="s">
         <v>25</v>
       </c>
       <c r="F40" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G40" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H40" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G40" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H40" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I40" s="35"/>
       <c r="J40" s="58"/>
@@ -3652,7 +3612,7 @@
     </row>
     <row r="41" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B41" s="19">
         <v>39</v>
@@ -3660,20 +3620,20 @@
       <c r="C41" s="28">
         <v>1</v>
       </c>
-      <c r="D41" s="63" t="s">
+      <c r="D41" s="28" t="s">
         <v>12</v>
       </c>
       <c r="E41" s="62" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F41" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G41" s="28" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H41" s="28" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I41" s="35"/>
       <c r="J41" s="59">
@@ -3684,12 +3644,12 @@
         <v>0.18551999999999999</v>
       </c>
       <c r="L41" s="33" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B42" s="19">
         <v>40</v>
@@ -3697,20 +3657,20 @@
       <c r="C42" s="28">
         <v>7</v>
       </c>
-      <c r="D42" s="63" t="s">
-        <v>250</v>
+      <c r="D42" s="28" t="s">
+        <v>244</v>
       </c>
       <c r="E42" s="28" t="s">
         <v>29</v>
       </c>
       <c r="F42" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G42" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H42" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G42" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H42" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I42" s="35"/>
       <c r="J42" s="59"/>
@@ -3722,7 +3682,7 @@
     </row>
     <row r="43" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B43" s="19">
         <v>41</v>
@@ -3730,20 +3690,20 @@
       <c r="C43" s="28">
         <v>7</v>
       </c>
-      <c r="D43" s="63" t="s">
+      <c r="D43" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="E43" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="E43" s="28" t="s">
-        <v>129</v>
-      </c>
       <c r="F43" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G43" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H43" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G43" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H43" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I43" s="38"/>
       <c r="J43" s="59"/>
@@ -3755,7 +3715,7 @@
     </row>
     <row r="44" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B44" s="19">
         <v>42</v>
@@ -3763,20 +3723,20 @@
       <c r="C44" s="28">
         <v>6</v>
       </c>
-      <c r="D44" s="63" t="s">
-        <v>248</v>
+      <c r="D44" s="28" t="s">
+        <v>242</v>
       </c>
       <c r="E44" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F44" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G44" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H44" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G44" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H44" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I44" s="35"/>
       <c r="J44" s="59"/>
@@ -3788,7 +3748,7 @@
     </row>
     <row r="45" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B45" s="19">
         <v>43</v>
@@ -3796,20 +3756,20 @@
       <c r="C45" s="28">
         <v>6</v>
       </c>
-      <c r="D45" s="63" t="s">
-        <v>249</v>
+      <c r="D45" s="28" t="s">
+        <v>243</v>
       </c>
       <c r="E45" s="28" t="s">
         <v>21</v>
       </c>
       <c r="F45" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G45" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H45" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G45" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H45" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I45" s="38"/>
       <c r="J45" s="59"/>
@@ -3821,7 +3781,7 @@
     </row>
     <row r="46" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B46" s="19">
         <v>44</v>
@@ -3829,20 +3789,20 @@
       <c r="C46" s="28">
         <v>7</v>
       </c>
-      <c r="D46" s="63" t="s">
-        <v>174</v>
+      <c r="D46" s="28" t="s">
+        <v>171</v>
       </c>
       <c r="E46" s="28" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F46" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G46" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H46" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G46" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H46" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I46" s="38"/>
       <c r="J46" s="59"/>
@@ -3854,7 +3814,7 @@
     </row>
     <row r="47" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B47" s="19">
         <v>45</v>
@@ -3862,20 +3822,20 @@
       <c r="C47" s="28">
         <v>2</v>
       </c>
-      <c r="D47" s="63" t="s">
-        <v>169</v>
+      <c r="D47" s="28" t="s">
+        <v>166</v>
       </c>
       <c r="E47" s="28" t="s">
         <v>16</v>
       </c>
       <c r="F47" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G47" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H47" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G47" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H47" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I47" s="35"/>
       <c r="J47" s="59"/>
@@ -3887,7 +3847,7 @@
     </row>
     <row r="48" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B48" s="19">
         <v>46</v>
@@ -3895,20 +3855,20 @@
       <c r="C48" s="28">
         <v>2</v>
       </c>
-      <c r="D48" s="63" t="s">
-        <v>171</v>
+      <c r="D48" s="28" t="s">
+        <v>168</v>
       </c>
       <c r="E48" s="28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F48" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G48" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H48" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G48" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H48" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I48" s="38"/>
       <c r="J48" s="59"/>
@@ -3918,42 +3878,27 @@
       </c>
       <c r="L48" s="47"/>
     </row>
-    <row r="49" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A49" s="18" t="s">
-        <v>73</v>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A49" s="19" t="s">
+        <v>69</v>
       </c>
       <c r="B49" s="19">
-        <v>47</v>
-      </c>
-      <c r="C49" s="28">
-        <v>2</v>
-      </c>
-      <c r="D49" s="63" t="s">
-        <v>132</v>
-      </c>
-      <c r="E49" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="F49" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="G49" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H49" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="I49" s="38"/>
+        <v>18</v>
+      </c>
+      <c r="C49" s="66"/>
+      <c r="D49" s="66"/>
+      <c r="E49" s="66"/>
+      <c r="F49" s="66"/>
+      <c r="G49" s="66"/>
+      <c r="H49" s="66"/>
+      <c r="I49" s="37"/>
       <c r="J49" s="58"/>
-      <c r="K49" s="58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L49" s="47"/>
+      <c r="K49" s="58"/>
+      <c r="L49" s="56"/>
     </row>
     <row r="50" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B50" s="19">
         <v>48</v>
@@ -3961,20 +3906,20 @@
       <c r="C50" s="28">
         <v>1</v>
       </c>
-      <c r="D50" s="63" t="s">
+      <c r="D50" s="28" t="s">
         <v>42</v>
       </c>
       <c r="E50" s="28" t="s">
         <v>41</v>
       </c>
       <c r="F50" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G50" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H50" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G50" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H50" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I50" s="35"/>
       <c r="J50" s="58"/>
@@ -3986,28 +3931,28 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B51" s="19">
         <v>49</v>
       </c>
-      <c r="C51" s="74">
+      <c r="C51" s="66">
         <v>0</v>
       </c>
-      <c r="D51" s="74" t="s">
-        <v>165</v>
-      </c>
-      <c r="E51" s="74" t="s">
-        <v>165</v>
-      </c>
-      <c r="F51" s="74" t="s">
-        <v>165</v>
-      </c>
-      <c r="G51" s="74" t="s">
-        <v>176</v>
-      </c>
-      <c r="H51" s="74" t="s">
-        <v>165</v>
+      <c r="D51" s="66" t="s">
+        <v>162</v>
+      </c>
+      <c r="E51" s="66" t="s">
+        <v>162</v>
+      </c>
+      <c r="F51" s="66" t="s">
+        <v>162</v>
+      </c>
+      <c r="G51" s="66" t="s">
+        <v>173</v>
+      </c>
+      <c r="H51" s="66" t="s">
+        <v>162</v>
       </c>
       <c r="I51" s="35"/>
       <c r="J51" s="58"/>
@@ -4019,7 +3964,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B52" s="19">
         <v>50</v>
@@ -4027,20 +3972,20 @@
       <c r="C52" s="28">
         <v>1</v>
       </c>
-      <c r="D52" s="63" t="s">
-        <v>168</v>
+      <c r="D52" s="28" t="s">
+        <v>165</v>
       </c>
       <c r="E52" s="28" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F52" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G52" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H52" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G52" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H52" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I52" s="40"/>
       <c r="J52" s="60"/>
@@ -4052,7 +3997,7 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B53" s="19">
         <v>51</v>
@@ -4060,20 +4005,20 @@
       <c r="C53" s="28">
         <v>1</v>
       </c>
-      <c r="D53" s="63" t="s">
+      <c r="D53" s="28" t="s">
         <v>34</v>
       </c>
       <c r="E53" s="28" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F53" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G53" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H53" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G53" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H53" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I53" s="40"/>
       <c r="J53" s="60"/>
@@ -4085,17 +4030,17 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B54" s="19">
         <v>52</v>
       </c>
-      <c r="C54" s="74"/>
-      <c r="D54" s="74"/>
-      <c r="E54" s="74"/>
-      <c r="F54" s="74"/>
-      <c r="G54" s="74"/>
-      <c r="H54" s="74"/>
+      <c r="C54" s="66"/>
+      <c r="D54" s="66"/>
+      <c r="E54" s="66"/>
+      <c r="F54" s="66"/>
+      <c r="G54" s="66"/>
+      <c r="H54" s="66"/>
       <c r="I54" s="40"/>
       <c r="J54" s="60"/>
       <c r="K54" s="58">
@@ -4106,7 +4051,7 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B55" s="19">
         <v>53</v>
@@ -4114,20 +4059,20 @@
       <c r="C55" s="28">
         <v>1</v>
       </c>
-      <c r="D55" s="63" t="s">
+      <c r="D55" s="28" t="s">
         <v>31</v>
       </c>
       <c r="E55" s="28" t="s">
         <v>30</v>
       </c>
       <c r="F55" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G55" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H55" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G55" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H55" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I55" s="40"/>
       <c r="J55" s="60"/>
@@ -4139,7 +4084,7 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B56" s="19">
         <v>54</v>
@@ -4147,20 +4092,20 @@
       <c r="C56" s="28">
         <v>1</v>
       </c>
-      <c r="D56" s="63" t="s">
+      <c r="D56" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="E56" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="E56" s="28" t="s">
-        <v>82</v>
-      </c>
       <c r="F56" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G56" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H56" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G56" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H56" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I56" s="42"/>
       <c r="J56" s="60"/>
@@ -4172,7 +4117,7 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B57" s="19">
         <v>55</v>
@@ -4180,20 +4125,20 @@
       <c r="C57" s="28">
         <v>1</v>
       </c>
-      <c r="D57" s="63" t="s">
-        <v>136</v>
+      <c r="D57" s="28" t="s">
+        <v>133</v>
       </c>
       <c r="E57" s="28" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F57" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G57" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H57" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G57" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H57" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I57" s="42"/>
       <c r="J57" s="60"/>
@@ -4205,17 +4150,17 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B58" s="19">
         <v>56</v>
       </c>
-      <c r="C58" s="74"/>
-      <c r="D58" s="74"/>
-      <c r="E58" s="74"/>
-      <c r="F58" s="74"/>
-      <c r="G58" s="74"/>
-      <c r="H58" s="74"/>
+      <c r="C58" s="66"/>
+      <c r="D58" s="66"/>
+      <c r="E58" s="66"/>
+      <c r="F58" s="66"/>
+      <c r="G58" s="66"/>
+      <c r="H58" s="66"/>
       <c r="I58" s="42"/>
       <c r="J58" s="60"/>
       <c r="K58" s="58">
@@ -4226,28 +4171,28 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B59" s="19">
         <v>57</v>
       </c>
-      <c r="C59" s="74">
+      <c r="C59" s="66">
         <v>0</v>
       </c>
-      <c r="D59" s="74" t="s">
-        <v>165</v>
-      </c>
-      <c r="E59" s="74" t="s">
-        <v>165</v>
-      </c>
-      <c r="F59" s="74" t="s">
-        <v>165</v>
-      </c>
-      <c r="G59" s="74" t="s">
-        <v>176</v>
-      </c>
-      <c r="H59" s="74" t="s">
-        <v>165</v>
+      <c r="D59" s="66" t="s">
+        <v>162</v>
+      </c>
+      <c r="E59" s="66" t="s">
+        <v>162</v>
+      </c>
+      <c r="F59" s="66" t="s">
+        <v>162</v>
+      </c>
+      <c r="G59" s="66" t="s">
+        <v>173</v>
+      </c>
+      <c r="H59" s="66" t="s">
+        <v>162</v>
       </c>
       <c r="I59" s="42"/>
       <c r="J59" s="60"/>
@@ -4259,7 +4204,7 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B60" s="19">
         <v>58</v>
@@ -4267,20 +4212,20 @@
       <c r="C60" s="28">
         <v>1</v>
       </c>
-      <c r="D60" s="63" t="s">
+      <c r="D60" s="28" t="s">
         <v>23</v>
       </c>
       <c r="E60" s="28" t="s">
         <v>22</v>
       </c>
       <c r="F60" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G60" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H60" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G60" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H60" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I60" s="42"/>
       <c r="J60" s="60"/>
@@ -4292,17 +4237,17 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B61" s="19">
         <v>59</v>
       </c>
-      <c r="C61" s="74"/>
-      <c r="D61" s="74"/>
-      <c r="E61" s="74"/>
-      <c r="F61" s="74"/>
-      <c r="G61" s="74"/>
-      <c r="H61" s="74"/>
+      <c r="C61" s="66"/>
+      <c r="D61" s="66"/>
+      <c r="E61" s="66"/>
+      <c r="F61" s="66"/>
+      <c r="G61" s="66"/>
+      <c r="H61" s="66"/>
       <c r="I61" s="42"/>
       <c r="J61" s="60"/>
       <c r="K61" s="58">
@@ -4313,7 +4258,7 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B62" s="19">
         <v>60</v>
@@ -4321,20 +4266,20 @@
       <c r="C62" s="28">
         <v>1</v>
       </c>
-      <c r="D62" s="63" t="s">
+      <c r="D62" s="28" t="s">
         <v>20</v>
       </c>
       <c r="E62" s="28" t="s">
         <v>19</v>
       </c>
       <c r="F62" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G62" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H62" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G62" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H62" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I62" s="42"/>
       <c r="J62" s="60"/>
@@ -4346,7 +4291,7 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B63" s="19">
         <v>61</v>
@@ -4354,20 +4299,20 @@
       <c r="C63" s="28">
         <v>1</v>
       </c>
-      <c r="D63" s="63" t="s">
+      <c r="D63" s="28" t="s">
         <v>47</v>
       </c>
       <c r="E63" s="28" t="s">
         <v>46</v>
       </c>
       <c r="F63" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G63" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H63" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G63" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H63" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I63" s="42"/>
       <c r="J63" s="60"/>
@@ -4379,7 +4324,7 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B64" s="19">
         <v>62</v>
@@ -4387,20 +4332,20 @@
       <c r="C64" s="28">
         <v>1</v>
       </c>
-      <c r="D64" s="63" t="s">
+      <c r="D64" s="28" t="s">
         <v>40</v>
       </c>
       <c r="E64" s="28" t="s">
         <v>39</v>
       </c>
       <c r="F64" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G64" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H64" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G64" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H64" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I64" s="42"/>
       <c r="J64" s="60"/>
@@ -4412,7 +4357,7 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B65" s="19">
         <v>63</v>
@@ -4420,20 +4365,20 @@
       <c r="C65" s="28">
         <v>1</v>
       </c>
-      <c r="D65" s="63" t="s">
-        <v>154</v>
+      <c r="D65" s="28" t="s">
+        <v>151</v>
       </c>
       <c r="E65" s="28" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F65" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G65" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H65" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G65" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H65" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I65" s="42"/>
       <c r="J65" s="60"/>
@@ -4445,17 +4390,17 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B66" s="19">
         <v>64</v>
       </c>
-      <c r="C66" s="74"/>
-      <c r="D66" s="74"/>
-      <c r="E66" s="75"/>
-      <c r="F66" s="74"/>
-      <c r="G66" s="74"/>
-      <c r="H66" s="74"/>
+      <c r="C66" s="66"/>
+      <c r="D66" s="66"/>
+      <c r="E66" s="67"/>
+      <c r="F66" s="66"/>
+      <c r="G66" s="66"/>
+      <c r="H66" s="66"/>
       <c r="I66" s="40"/>
       <c r="J66" s="60">
         <v>6.2199999999999998E-2</v>
@@ -4465,12 +4410,12 @@
         <v>0</v>
       </c>
       <c r="L66" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B67" s="19">
         <v>65</v>
@@ -4478,20 +4423,20 @@
       <c r="C67" s="28">
         <v>1</v>
       </c>
-      <c r="D67" s="63" t="s">
-        <v>68</v>
+      <c r="D67" s="28" t="s">
+        <v>67</v>
       </c>
       <c r="E67" s="28" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F67" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G67" s="28" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H67" s="28" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="I67" s="40"/>
       <c r="J67" s="60">
@@ -4502,12 +4447,12 @@
         <v>0.91432999999999998</v>
       </c>
       <c r="L67" s="50" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B68" s="19">
         <v>66</v>
@@ -4515,20 +4460,20 @@
       <c r="C68" s="28">
         <v>1</v>
       </c>
-      <c r="D68" s="63" t="s">
+      <c r="D68" s="28" t="s">
         <v>8</v>
       </c>
       <c r="E68" s="28" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F68" s="28" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="G68" s="28" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H68" s="28" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="I68" s="40"/>
       <c r="J68" s="60">
@@ -4539,12 +4484,12 @@
         <v>0.53656000000000004</v>
       </c>
       <c r="L68" s="50" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B69" s="19">
         <v>67</v>
@@ -4552,20 +4497,20 @@
       <c r="C69" s="28">
         <v>1</v>
       </c>
-      <c r="D69" s="63" t="s">
+      <c r="D69" s="28" t="s">
         <v>48</v>
       </c>
       <c r="E69" s="28" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F69" s="28" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G69" s="28" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H69" s="28" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I69" s="40"/>
       <c r="J69" s="60">
@@ -4576,22 +4521,22 @@
         <v>0.65</v>
       </c>
       <c r="L69" s="50" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B70" s="19">
         <v>68</v>
       </c>
-      <c r="C70" s="74"/>
-      <c r="D70" s="74"/>
-      <c r="E70" s="74"/>
-      <c r="F70" s="74"/>
-      <c r="G70" s="74"/>
-      <c r="H70" s="74"/>
+      <c r="C70" s="66"/>
+      <c r="D70" s="66"/>
+      <c r="E70" s="66"/>
+      <c r="F70" s="66"/>
+      <c r="G70" s="66"/>
+      <c r="H70" s="66"/>
       <c r="I70" s="40"/>
       <c r="J70" s="60"/>
       <c r="K70" s="58">
@@ -4601,7 +4546,7 @@
     </row>
     <row r="71" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="51" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B71" s="19">
         <v>69</v>
@@ -4609,20 +4554,20 @@
       <c r="C71" s="28">
         <v>1</v>
       </c>
-      <c r="D71" s="63" t="s">
-        <v>139</v>
+      <c r="D71" s="28" t="s">
+        <v>136</v>
       </c>
       <c r="E71" s="28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F71" s="28" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G71" s="28" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H71" s="28" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I71" s="40"/>
       <c r="J71" s="60">
@@ -4633,12 +4578,12 @@
         <v>0.42686000000000002</v>
       </c>
       <c r="L71" s="50" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B72" s="19">
         <v>70</v>
@@ -4646,20 +4591,20 @@
       <c r="C72" s="28">
         <v>1</v>
       </c>
-      <c r="D72" s="63" t="s">
-        <v>142</v>
+      <c r="D72" s="28" t="s">
+        <v>139</v>
       </c>
       <c r="E72" s="28" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F72" s="28" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G72" s="28" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H72" s="28" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I72" s="43"/>
       <c r="J72" s="59">
@@ -4670,12 +4615,12 @@
         <v>1.2505999999999999</v>
       </c>
       <c r="L72" s="46" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B73" s="19">
         <v>71</v>
@@ -4683,20 +4628,20 @@
       <c r="C73" s="28">
         <v>0</v>
       </c>
-      <c r="D73" s="63" t="s">
+      <c r="D73" s="28" t="s">
         <v>6</v>
       </c>
       <c r="E73" s="28" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F73" s="28" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G73" s="28" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H73" s="28" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I73" s="40"/>
       <c r="J73" s="60"/>
@@ -4705,12 +4650,12 @@
         <v>0</v>
       </c>
       <c r="L73" s="57" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B74" s="19">
         <v>72</v>
@@ -4718,17 +4663,17 @@
       <c r="C74" s="28">
         <v>2</v>
       </c>
-      <c r="D74" s="63" t="s">
+      <c r="D74" s="28" t="s">
         <v>44</v>
       </c>
       <c r="E74" s="28" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F74" s="28">
         <v>7414</v>
       </c>
       <c r="G74" s="28" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H74" s="28" t="s">
         <v>45</v>
@@ -4742,12 +4687,12 @@
         <v>0.54127999999999998</v>
       </c>
       <c r="L74" s="50" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B75" s="19">
         <v>73</v>
@@ -4755,20 +4700,20 @@
       <c r="C75" s="28">
         <v>1</v>
       </c>
-      <c r="D75" s="63" t="s">
-        <v>62</v>
+      <c r="D75" s="28" t="s">
+        <v>61</v>
       </c>
       <c r="E75" s="28" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F75" s="28" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G75" s="28" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H75" s="28" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I75" s="41"/>
       <c r="J75" s="60">
@@ -4779,12 +4724,12 @@
         <v>1.0848</v>
       </c>
       <c r="L75" s="50" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B76" s="19">
         <v>74</v>
@@ -4792,20 +4737,20 @@
       <c r="C76" s="28">
         <v>1</v>
       </c>
-      <c r="D76" s="63" t="s">
-        <v>58</v>
+      <c r="D76" s="28" t="s">
+        <v>57</v>
       </c>
       <c r="E76" s="28" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F76" s="28" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G76" s="28" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="H76" s="28" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I76" s="40"/>
       <c r="J76" s="60">
@@ -4816,12 +4761,12 @@
         <v>0.75968000000000002</v>
       </c>
       <c r="L76" s="50" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B77" s="19">
         <v>75</v>
@@ -4829,7 +4774,7 @@
       <c r="C77" s="28">
         <v>1</v>
       </c>
-      <c r="D77" s="63" t="s">
+      <c r="D77" s="28" t="s">
         <v>10</v>
       </c>
       <c r="E77" s="28" t="s">
@@ -4839,7 +4784,7 @@
         <v>9</v>
       </c>
       <c r="G77" s="28" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="H77" s="28"/>
       <c r="I77" s="40"/>
@@ -4851,12 +4796,12 @@
         <v>1.02728</v>
       </c>
       <c r="L77" s="50" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B78" s="19">
         <v>76</v>
@@ -4864,20 +4809,20 @@
       <c r="C78" s="28">
         <v>1</v>
       </c>
-      <c r="D78" s="63" t="s">
+      <c r="D78" s="28" t="s">
         <v>11</v>
       </c>
       <c r="E78" s="28" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F78" s="28" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G78" s="28" t="s">
         <v>50</v>
       </c>
       <c r="H78" s="28" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="I78" s="40"/>
       <c r="J78" s="60">
@@ -4888,22 +4833,22 @@
         <v>0.28182000000000001</v>
       </c>
       <c r="L78" s="50" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B79" s="19">
         <v>77</v>
       </c>
-      <c r="C79" s="74"/>
-      <c r="D79" s="74"/>
-      <c r="E79" s="74"/>
-      <c r="F79" s="74"/>
-      <c r="G79" s="74"/>
-      <c r="H79" s="74"/>
+      <c r="C79" s="66"/>
+      <c r="D79" s="66"/>
+      <c r="E79" s="66"/>
+      <c r="F79" s="66"/>
+      <c r="G79" s="66"/>
+      <c r="H79" s="66"/>
       <c r="I79" s="40"/>
       <c r="J79" s="60">
         <v>0.86136000000000001</v>
@@ -4913,12 +4858,12 @@
         <v>0</v>
       </c>
       <c r="L79" s="50" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B80" s="19">
         <v>78</v>
@@ -4926,20 +4871,20 @@
       <c r="C80" s="28">
         <v>1</v>
       </c>
-      <c r="D80" s="63" t="s">
+      <c r="D80" s="28" t="s">
         <v>18</v>
       </c>
       <c r="E80" s="28" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F80" s="28" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G80" s="28" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H80" s="28" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I80" s="40"/>
       <c r="J80" s="60">
@@ -4950,12 +4895,12 @@
         <v>0.57067999999999997</v>
       </c>
       <c r="L80" s="50" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B81" s="19">
         <v>79</v>
@@ -4963,20 +4908,20 @@
       <c r="C81" s="28">
         <v>1</v>
       </c>
-      <c r="D81" s="65" t="s">
-        <v>159</v>
+      <c r="D81" s="64" t="s">
+        <v>156</v>
       </c>
       <c r="E81" s="44" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F81" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G81" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H81" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G81" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H81" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I81" s="40"/>
       <c r="J81" s="60"/>
@@ -4987,7 +4932,7 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B82" s="19">
         <v>80</v>
@@ -4995,11 +4940,11 @@
       <c r="C82" s="28">
         <v>0</v>
       </c>
-      <c r="D82" s="65" t="s">
-        <v>160</v>
+      <c r="D82" s="64" t="s">
+        <v>157</v>
       </c>
       <c r="E82" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F82" s="28" t="s">
         <v>49</v>
@@ -5020,7 +4965,7 @@
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B83" s="19">
         <v>81</v>
@@ -5028,20 +4973,20 @@
       <c r="C83" s="28">
         <v>1</v>
       </c>
-      <c r="D83" s="63" t="s">
+      <c r="D83" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="E83" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="F83" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G83" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="E83" s="28" t="s">
-        <v>170</v>
-      </c>
-      <c r="F83" s="28" t="s">
+      <c r="H83" s="28" t="s">
         <v>125</v>
-      </c>
-      <c r="G83" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="H83" s="28" t="s">
-        <v>126</v>
       </c>
       <c r="I83" s="40"/>
       <c r="J83" s="60"/>
@@ -5055,11 +5000,11 @@
       <c r="G84" s="45"/>
       <c r="J84" s="61">
         <f>SUM(J7:J83)</f>
-        <v>13.288069999999996</v>
+        <v>13.179349999999998</v>
       </c>
       <c r="K84" s="61">
         <f>SUM(K7:K83)</f>
-        <v>12.826489999999998</v>
+        <v>12.717769999999998</v>
       </c>
     </row>
   </sheetData>
@@ -5086,24 +5031,23 @@
     <hyperlink ref="L28" r:id="rId11" xr:uid="{518A6692-3A50-F942-B48D-CC4356762EAD}"/>
     <hyperlink ref="L22" r:id="rId12" xr:uid="{A1379108-F295-EE45-B6ED-5162031D55EB}"/>
     <hyperlink ref="L7" r:id="rId13" xr:uid="{5948B746-AAC4-5740-AB8C-E151299C82FE}"/>
-    <hyperlink ref="L21" r:id="rId14" xr:uid="{7F2AFDE5-1B48-DB4E-A5DC-FF059C0FC2B5}"/>
-    <hyperlink ref="L24" r:id="rId15" xr:uid="{646B658D-AE56-44EA-A58F-40CDBDEF2D0C}"/>
-    <hyperlink ref="L26" r:id="rId16" xr:uid="{47FDBB7E-44E8-4353-9597-0562E7BF59F5}"/>
-    <hyperlink ref="L27" r:id="rId17" xr:uid="{8736A480-3930-45F7-AECD-F285FFC9909F}"/>
-    <hyperlink ref="L30" r:id="rId18" xr:uid="{F9FA5EE5-1B77-4F3B-8F3F-3842AA6F0BAA}"/>
-    <hyperlink ref="L33" r:id="rId19" xr:uid="{AB84C394-095B-406A-966B-81DF3D2E2812}"/>
-    <hyperlink ref="L31" r:id="rId20" xr:uid="{C8A6F598-6C7B-4E81-A0E7-EBB0B449E508}"/>
-    <hyperlink ref="L32" r:id="rId21" xr:uid="{51DB6C5F-D3B9-4DE7-B2D3-FC15FA2E815B}"/>
-    <hyperlink ref="L34" r:id="rId22" xr:uid="{1E8D4B86-2BB1-4BC4-B74E-EFE1D1B71B87}"/>
-    <hyperlink ref="L37" r:id="rId23" xr:uid="{E3611F41-7D12-4600-84CB-E5DA78E4D275}"/>
-    <hyperlink ref="L38" r:id="rId24" xr:uid="{F8FD3DE4-2053-469C-A880-F854815B0BBC}"/>
-    <hyperlink ref="L67" r:id="rId25" xr:uid="{5E58DFC9-92C6-487D-82FB-789F079E9373}"/>
-    <hyperlink ref="L68" r:id="rId26" xr:uid="{9D884BB0-E9D5-416B-B348-A3CCA307ED67}"/>
-    <hyperlink ref="L73" r:id="rId27" xr:uid="{4AD4981F-0482-460C-B12B-D6E5A82469EE}"/>
-    <hyperlink ref="L78" r:id="rId28" xr:uid="{168580DB-C131-4BC7-9E3D-A9AEB4A7EE65}"/>
+    <hyperlink ref="L24" r:id="rId14" xr:uid="{646B658D-AE56-44EA-A58F-40CDBDEF2D0C}"/>
+    <hyperlink ref="L26" r:id="rId15" xr:uid="{47FDBB7E-44E8-4353-9597-0562E7BF59F5}"/>
+    <hyperlink ref="L27" r:id="rId16" xr:uid="{8736A480-3930-45F7-AECD-F285FFC9909F}"/>
+    <hyperlink ref="L30" r:id="rId17" xr:uid="{F9FA5EE5-1B77-4F3B-8F3F-3842AA6F0BAA}"/>
+    <hyperlink ref="L33" r:id="rId18" xr:uid="{AB84C394-095B-406A-966B-81DF3D2E2812}"/>
+    <hyperlink ref="L31" r:id="rId19" xr:uid="{C8A6F598-6C7B-4E81-A0E7-EBB0B449E508}"/>
+    <hyperlink ref="L32" r:id="rId20" xr:uid="{51DB6C5F-D3B9-4DE7-B2D3-FC15FA2E815B}"/>
+    <hyperlink ref="L34" r:id="rId21" xr:uid="{1E8D4B86-2BB1-4BC4-B74E-EFE1D1B71B87}"/>
+    <hyperlink ref="L37" r:id="rId22" xr:uid="{E3611F41-7D12-4600-84CB-E5DA78E4D275}"/>
+    <hyperlink ref="L38" r:id="rId23" xr:uid="{F8FD3DE4-2053-469C-A880-F854815B0BBC}"/>
+    <hyperlink ref="L67" r:id="rId24" xr:uid="{5E58DFC9-92C6-487D-82FB-789F079E9373}"/>
+    <hyperlink ref="L68" r:id="rId25" xr:uid="{9D884BB0-E9D5-416B-B348-A3CCA307ED67}"/>
+    <hyperlink ref="L73" r:id="rId26" xr:uid="{4AD4981F-0482-460C-B12B-D6E5A82469EE}"/>
+    <hyperlink ref="L78" r:id="rId27" xr:uid="{168580DB-C131-4BC7-9E3D-A9AEB4A7EE65}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
 
@@ -5111,10 +5055,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="1">
+    <sheetView topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="1">
       <selection activeCell="C4" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
@@ -5127,7 +5071,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1"/>
     </row>
@@ -5137,38 +5081,38 @@
     </row>
     <row r="3" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D3" s="53" t="s">
         <v>78</v>
-      </c>
-      <c r="D3" s="53" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="68" t="s">
-        <v>157</v>
-      </c>
-      <c r="B4" s="69">
-        <v>45020</v>
-      </c>
-      <c r="C4" s="70" t="s">
-        <v>156</v>
+        <v>154</v>
+      </c>
+      <c r="B4" s="70">
+        <v>45246</v>
+      </c>
+      <c r="C4" s="72" t="s">
+        <v>153</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="204" x14ac:dyDescent="0.2">
-      <c r="A5" s="71"/>
-      <c r="B5" s="72"/>
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="229.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="69"/>
+      <c r="B5" s="71"/>
       <c r="C5" s="73"/>
       <c r="D5" s="34" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>